<commit_message>
linear search test description added
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -295,6 +295,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFCD184"/>
       <color rgb="FFE8DD4E"/>
       <color rgb="FFEAEE48"/>
       <color rgb="FFA365D1"/>
@@ -7508,8 +7509,167 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>target_performance</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FCD184"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'linear search'!$O$6:$O$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'linear search'!$Q$6:$Q$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>436</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>linear search</c:v>
           </c:tx>
@@ -7922,6 +8082,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId1"/>
 </c:chartSpace>
 </file>
 
@@ -13585,6 +13746,46 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.81126</cdr:x>
+      <cdr:y>0.68609</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.96195</cdr:x>
+      <cdr:y>0.75455</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6769100" y="2990850"/>
+          <a:ext cx="1257300" cy="298450"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="800"/>
+            <a:t>target performance = 436 </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -20206,10 +20407,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="O5:P33"/>
+  <dimension ref="O5:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20217,7 +20418,7 @@
     <col min="16" max="16" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="15:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O5" t="s">
         <v>49</v>
       </c>
@@ -20225,167 +20426,227 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="15:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O6">
         <v>10</v>
       </c>
       <c r="P6">
         <v>136</v>
       </c>
-    </row>
-    <row r="7" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q6">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="7" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O7">
         <v>50</v>
       </c>
       <c r="P7">
         <v>164</v>
       </c>
-    </row>
-    <row r="8" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q7">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="8" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O8">
         <v>100</v>
       </c>
       <c r="P8">
         <v>207</v>
       </c>
-    </row>
-    <row r="9" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q8">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="9" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O9">
         <v>200</v>
       </c>
       <c r="P9">
         <v>279</v>
       </c>
-    </row>
-    <row r="10" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q9">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="10" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O10">
         <v>300</v>
       </c>
       <c r="P10">
         <v>350</v>
       </c>
-    </row>
-    <row r="11" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q10">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="11" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O11">
         <v>400</v>
       </c>
       <c r="P11">
         <v>422</v>
       </c>
-    </row>
-    <row r="12" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q11">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="12" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O12">
         <v>500</v>
       </c>
       <c r="P12">
         <v>493</v>
       </c>
-    </row>
-    <row r="13" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q12">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="13" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O13">
         <v>600</v>
       </c>
       <c r="P13">
         <v>563</v>
       </c>
-    </row>
-    <row r="14" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q13">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="14" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O14">
         <v>700</v>
       </c>
       <c r="P14">
         <v>636</v>
       </c>
-    </row>
-    <row r="15" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q14">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="15" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O15">
         <v>800</v>
       </c>
       <c r="P15">
         <v>712</v>
       </c>
-    </row>
-    <row r="16" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q15">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="16" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O16">
         <v>900</v>
       </c>
       <c r="P16">
         <v>791</v>
       </c>
-    </row>
-    <row r="17" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q16">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="17" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O17">
         <v>1000</v>
       </c>
       <c r="P17">
         <v>849</v>
       </c>
-    </row>
-    <row r="18" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q17">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="18" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O18">
         <v>1100</v>
       </c>
       <c r="P18">
         <v>936</v>
       </c>
-    </row>
-    <row r="19" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q18">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="19" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O19">
         <v>1200</v>
       </c>
       <c r="P19">
         <v>993</v>
       </c>
-    </row>
-    <row r="20" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q19">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="20" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O20">
         <v>1300</v>
       </c>
       <c r="P20">
         <v>1061</v>
       </c>
-    </row>
-    <row r="21" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q20">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="21" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O21">
         <v>1400</v>
       </c>
       <c r="P21">
         <v>1139</v>
       </c>
-    </row>
-    <row r="22" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q21">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="22" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O22">
         <v>1500</v>
       </c>
       <c r="P22">
         <v>1208</v>
       </c>
-    </row>
-    <row r="23" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q22">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="23" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O23">
         <v>1600</v>
       </c>
       <c r="P23">
         <v>1279</v>
       </c>
-    </row>
-    <row r="24" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q23">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="24" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O24">
         <v>2000</v>
       </c>
       <c r="P24">
         <v>1561</v>
       </c>
-    </row>
-    <row r="25" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q24">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="25" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O25">
         <v>4000</v>
       </c>
       <c r="P25">
         <v>3006</v>
       </c>
-    </row>
-    <row r="26" spans="15:16" x14ac:dyDescent="0.35">
+      <c r="Q25">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="26" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O26">
         <v>6000</v>
       </c>
@@ -20393,7 +20654,7 @@
         <v>4444</v>
       </c>
     </row>
-    <row r="27" spans="15:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O27">
         <v>8000</v>
       </c>
@@ -20401,7 +20662,7 @@
         <v>5861</v>
       </c>
     </row>
-    <row r="28" spans="15:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O28">
         <v>10000</v>
       </c>
@@ -20409,7 +20670,7 @@
         <v>7338</v>
       </c>
     </row>
-    <row r="29" spans="15:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O29">
         <v>20000</v>
       </c>
@@ -20417,7 +20678,7 @@
         <v>15852</v>
       </c>
     </row>
-    <row r="30" spans="15:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O30">
         <v>30000</v>
       </c>
@@ -20425,7 +20686,7 @@
         <v>22741</v>
       </c>
     </row>
-    <row r="31" spans="15:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O31">
         <v>40000</v>
       </c>
@@ -20433,7 +20694,7 @@
         <v>31142</v>
       </c>
     </row>
-    <row r="32" spans="15:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O32">
         <v>50000</v>
       </c>

</xml_diff>

<commit_message>
beginning of the tree based nat table description added
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="110" windowWidth="14360" windowHeight="4680" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="110" windowWidth="14360" windowHeight="4680" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Ideal NAT" sheetId="3" r:id="rId3"/>
     <sheet name="linear search" sheetId="4" r:id="rId4"/>
+    <sheet name="tree_tree" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="51">
   <si>
     <t>n</t>
   </si>
@@ -8053,6 +8054,753 @@
           </a:ln>
         </c:spPr>
         <c:crossAx val="71793664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln cmpd="sng">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr anchor="t" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0"/>
+              <a:t>Nat Performance - Linear Search </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>CPU: i5-4210U, 1 core</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0"/>
+              <a:t>[cycles/packet]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.8471703696317515E-2"/>
+          <c:y val="1.2330720131214482E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.9429535280808154E-2"/>
+          <c:y val="0.23300827354297415"/>
+          <c:w val="0.8587591963900808"/>
+          <c:h val="0.66316192505535121"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>target_performance</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FCD184"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'linear search'!$O$6:$O$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'linear search'!$Q$6:$Q$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>436</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>linear search</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.4257962614360504E-2"/>
+                  <c:y val="1.944314134804526E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.6034712308957578E-3"/>
+                  <c:y val="1.6057716019292307E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.0346243404911767E-2"/>
+                  <c:y val="-3.657144823393798E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.1868313602549601E-2"/>
+                  <c:y val="-3.6665500570622303E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.0346243404911781E-2"/>
+                  <c:y val="-3.657121883799485E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:numFmt formatCode="0" sourceLinked="0"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'linear search'!$O$6:$O$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'linear search'!$P$6:$P$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>422</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>493</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>563</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>636</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>712</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>791</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>849</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>936</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>993</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1061</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1139</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1208</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1279</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1561</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3006</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4444</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5861</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7338</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>15852</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22741</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>31142</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40121</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>80154</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="126960768"/>
+        <c:axId val="126962688"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="126960768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2200"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                  <a:t>nat table size [entries]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.44666684004684143"/>
+              <c:y val="0.95213401310997814"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="126962688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="126962688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="22225">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="126960768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12978,6 +13726,46 @@
     <xdr:clientData/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.81126</cdr:x>
+      <cdr:y>0.68609</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.96195</cdr:x>
+      <cdr:y>0.75455</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6769100" y="2990850"/>
+          <a:ext cx="1257300" cy="298450"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="800"/>
+            <a:t>target performance = 436 </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13786,6 +14574,43 @@
 </c:userShapes>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -20409,8 +21234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="O5:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5:Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20714,4 +21539,264 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="O2:Q24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O3">
+        <v>10</v>
+      </c>
+      <c r="P3">
+        <v>136</v>
+      </c>
+      <c r="Q3">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="4" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O4">
+        <v>50</v>
+      </c>
+      <c r="P4">
+        <v>164</v>
+      </c>
+      <c r="Q4">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="5" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O5">
+        <v>100</v>
+      </c>
+      <c r="P5">
+        <v>207</v>
+      </c>
+      <c r="Q5">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="6" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O6">
+        <v>200</v>
+      </c>
+      <c r="P6">
+        <v>279</v>
+      </c>
+      <c r="Q6">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="7" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O7">
+        <v>300</v>
+      </c>
+      <c r="P7">
+        <v>350</v>
+      </c>
+      <c r="Q7">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="8" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O8">
+        <v>400</v>
+      </c>
+      <c r="P8">
+        <v>422</v>
+      </c>
+      <c r="Q8">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="9" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O9">
+        <v>500</v>
+      </c>
+      <c r="P9">
+        <v>493</v>
+      </c>
+      <c r="Q9">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="10" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O10">
+        <v>600</v>
+      </c>
+      <c r="P10">
+        <v>563</v>
+      </c>
+      <c r="Q10">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="11" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O11">
+        <v>700</v>
+      </c>
+      <c r="P11">
+        <v>636</v>
+      </c>
+      <c r="Q11">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="12" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O12">
+        <v>800</v>
+      </c>
+      <c r="P12">
+        <v>712</v>
+      </c>
+      <c r="Q12">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="13" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O13">
+        <v>900</v>
+      </c>
+      <c r="P13">
+        <v>791</v>
+      </c>
+      <c r="Q13">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="14" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O14">
+        <v>1000</v>
+      </c>
+      <c r="P14">
+        <v>849</v>
+      </c>
+      <c r="Q14">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="15" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O15">
+        <v>1100</v>
+      </c>
+      <c r="P15">
+        <v>936</v>
+      </c>
+      <c r="Q15">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="16" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O16">
+        <v>1200</v>
+      </c>
+      <c r="P16">
+        <v>993</v>
+      </c>
+      <c r="Q16">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="17" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O17">
+        <v>1300</v>
+      </c>
+      <c r="P17">
+        <v>1061</v>
+      </c>
+      <c r="Q17">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="18" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O18">
+        <v>1400</v>
+      </c>
+      <c r="P18">
+        <v>1139</v>
+      </c>
+      <c r="Q18">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="19" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O19">
+        <v>1500</v>
+      </c>
+      <c r="P19">
+        <v>1208</v>
+      </c>
+      <c r="Q19">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="20" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O20">
+        <v>1600</v>
+      </c>
+      <c r="P20">
+        <v>1279</v>
+      </c>
+      <c r="Q20">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="21" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O21">
+        <v>2000</v>
+      </c>
+      <c r="P21">
+        <v>1561</v>
+      </c>
+      <c r="Q21">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="22" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O22">
+        <v>4000</v>
+      </c>
+      <c r="P22">
+        <v>3006</v>
+      </c>
+      <c r="Q22">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="23" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O23">
+        <v>6000</v>
+      </c>
+      <c r="P23">
+        <v>4444</v>
+      </c>
+    </row>
+    <row r="24" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O24">
+        <v>8000</v>
+      </c>
+      <c r="P24">
+        <v>5861</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
binary tree based table added
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -8133,7 +8133,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0"/>
-              <a:t>Nat Performance - Linear Search </a:t>
+              <a:t>Nat Performance - Binary tree-based NAT table </a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -8224,7 +8224,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1100" b="0"/>
+              <a:rPr lang="en-US" sz="800" b="1"/>
               <a:t>[cycles/packet]</a:t>
             </a:r>
           </a:p>
@@ -8234,8 +8234,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8471703696317515E-2"/>
-          <c:y val="1.2330720131214482E-2"/>
+          <c:x val="3.4773071917577142E-2"/>
+          <c:y val="2.3984034042357966E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -8419,7 +8419,7 @@
           <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>linear search</c:v>
+            <c:v>binary tree</c:v>
           </c:tx>
           <c:spPr>
             <a:ln>
@@ -8454,8 +8454,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.4257962614360504E-2"/>
-                  <c:y val="1.944314134804526E-2"/>
+                  <c:x val="-1.1213822219084853E-2"/>
+                  <c:y val="-2.7170114296528665E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -8470,8 +8470,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.6034712308957578E-3"/>
-                  <c:y val="1.6057716019292307E-2"/>
+                  <c:x val="-1.8824173207273961E-2"/>
+                  <c:y val="-5.0948838969782716E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -8486,8 +8486,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.0346243404911767E-2"/>
-                  <c:y val="-3.657144823393798E-2"/>
+                  <c:x val="-3.404487518365204E-2"/>
+                  <c:y val="-2.2004805845008631E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -8530,7 +8530,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
             </c:dLbl>
-            <c:numFmt formatCode="0" sourceLinked="0"/>
+            <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -8552,159 +8552,36 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'linear search'!$O$6:$O$24</c:f>
+              <c:f>tree_tree!$O$3:$O$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1100</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1400</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1600</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'linear search'!$P$6:$P$33</c:f>
+              <c:f>tree_tree!$P$3:$P$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>136</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10522</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>164</c:v>
+                  <c:v>133550</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>207</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>279</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>422</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>493</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>563</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>636</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>712</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>791</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>849</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>936</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>993</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1061</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1139</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1208</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1279</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1561</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3006</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4444</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>5861</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7338</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>15852</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>22741</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>31142</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>40121</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>80154</c:v>
+                  <c:v>3769296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8727,7 +8604,6 @@
         <c:axId val="126960768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2200"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -8742,8 +8618,12 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="en-US" sz="800" baseline="0"/>
+                  <a:t>nat table size [entries</a:t>
+                </a:r>
+                <a:r>
                   <a:rPr lang="en-US" sz="1100" baseline="0"/>
-                  <a:t>nat table size [entries]</a:t>
+                  <a:t>]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -8752,13 +8632,13 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.44666684004684143"/>
-              <c:y val="0.95213401310997814"/>
+              <c:x val="0.83175060004920953"/>
+              <c:y val="0.84142753095411504"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
@@ -8770,6 +8650,16 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="126962688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -8778,6 +8668,8 @@
         <c:axId val="126962688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="4000000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -8790,7 +8682,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -8800,6 +8692,16 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="126960768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -13732,12 +13634,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.81126</cdr:x>
-      <cdr:y>0.68609</cdr:y>
+      <cdr:x>0.32268</cdr:x>
+      <cdr:y>0.84487</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.96195</cdr:x>
-      <cdr:y>0.75455</cdr:y>
+      <cdr:x>0.47337</cdr:x>
+      <cdr:y>0.91333</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -13746,8 +13648,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="6769100" y="2990850"/>
-          <a:ext cx="1257300" cy="298450"/>
+          <a:off x="2692372" y="3683005"/>
+          <a:ext cx="1257342" cy="298436"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -21234,7 +21136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="O5:Q33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="O5" sqref="O5:Q27"/>
     </sheetView>
   </sheetViews>
@@ -21543,10 +21445,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="O2:Q24"/>
+  <dimension ref="O2:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21561,10 +21463,10 @@
     </row>
     <row r="3" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O3">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="P3">
-        <v>136</v>
+        <v>10522</v>
       </c>
       <c r="Q3">
         <v>436</v>
@@ -21572,10 +21474,10 @@
     </row>
     <row r="4" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O4">
-        <v>50</v>
+        <v>10000</v>
       </c>
       <c r="P4">
-        <v>164</v>
+        <v>133550</v>
       </c>
       <c r="Q4">
         <v>436</v>
@@ -21583,216 +21485,13 @@
     </row>
     <row r="5" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O5">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="P5">
-        <v>207</v>
+        <v>3769296</v>
       </c>
       <c r="Q5">
         <v>436</v>
-      </c>
-    </row>
-    <row r="6" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O6">
-        <v>200</v>
-      </c>
-      <c r="P6">
-        <v>279</v>
-      </c>
-      <c r="Q6">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="7" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O7">
-        <v>300</v>
-      </c>
-      <c r="P7">
-        <v>350</v>
-      </c>
-      <c r="Q7">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="8" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O8">
-        <v>400</v>
-      </c>
-      <c r="P8">
-        <v>422</v>
-      </c>
-      <c r="Q8">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="9" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O9">
-        <v>500</v>
-      </c>
-      <c r="P9">
-        <v>493</v>
-      </c>
-      <c r="Q9">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="10" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O10">
-        <v>600</v>
-      </c>
-      <c r="P10">
-        <v>563</v>
-      </c>
-      <c r="Q10">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="11" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O11">
-        <v>700</v>
-      </c>
-      <c r="P11">
-        <v>636</v>
-      </c>
-      <c r="Q11">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="12" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O12">
-        <v>800</v>
-      </c>
-      <c r="P12">
-        <v>712</v>
-      </c>
-      <c r="Q12">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="13" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O13">
-        <v>900</v>
-      </c>
-      <c r="P13">
-        <v>791</v>
-      </c>
-      <c r="Q13">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="14" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O14">
-        <v>1000</v>
-      </c>
-      <c r="P14">
-        <v>849</v>
-      </c>
-      <c r="Q14">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="15" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O15">
-        <v>1100</v>
-      </c>
-      <c r="P15">
-        <v>936</v>
-      </c>
-      <c r="Q15">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="16" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O16">
-        <v>1200</v>
-      </c>
-      <c r="P16">
-        <v>993</v>
-      </c>
-      <c r="Q16">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="17" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O17">
-        <v>1300</v>
-      </c>
-      <c r="P17">
-        <v>1061</v>
-      </c>
-      <c r="Q17">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="18" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O18">
-        <v>1400</v>
-      </c>
-      <c r="P18">
-        <v>1139</v>
-      </c>
-      <c r="Q18">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="19" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O19">
-        <v>1500</v>
-      </c>
-      <c r="P19">
-        <v>1208</v>
-      </c>
-      <c r="Q19">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="20" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O20">
-        <v>1600</v>
-      </c>
-      <c r="P20">
-        <v>1279</v>
-      </c>
-      <c r="Q20">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="21" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O21">
-        <v>2000</v>
-      </c>
-      <c r="P21">
-        <v>1561</v>
-      </c>
-      <c r="Q21">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="22" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O22">
-        <v>4000</v>
-      </c>
-      <c r="P22">
-        <v>3006</v>
-      </c>
-      <c r="Q22">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="23" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O23">
-        <v>6000</v>
-      </c>
-      <c r="P23">
-        <v>4444</v>
-      </c>
-    </row>
-    <row r="24" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O24">
-        <v>8000</v>
-      </c>
-      <c r="P24">
-        <v>5861</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a part of parallel processing  description added
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="110" windowWidth="14360" windowHeight="4680" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="110" windowWidth="14360" windowHeight="4680" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Ideal NAT" sheetId="3" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="tree_tree" sheetId="5" r:id="rId3"/>
     <sheet name="tree_array" sheetId="6" r:id="rId4"/>
     <sheet name="hash" sheetId="8" r:id="rId5"/>
+    <sheet name="parallel_hash" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>chesums+timestamp</t>
   </si>
@@ -33,6 +34,12 @@
   </si>
   <si>
     <t>cycles per packet</t>
+  </si>
+  <si>
+    <t>core</t>
+  </si>
+  <si>
+    <t>target</t>
   </si>
 </sst>
 </file>
@@ -69,8 +76,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3203,6 +3213,627 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr anchor="t" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0"/>
+              <a:t>Nat Performance - Hash-based NAT table</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>CPU: i5-4210U, 1 core</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="800" b="1"/>
+              <a:t>[cycles/packet]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.9126195079782243E-2"/>
+          <c:y val="2.1070705564572093E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.4863324687894712E-2"/>
+          <c:y val="0.23883489800482879"/>
+          <c:w val="0.8587591963900808"/>
+          <c:h val="0.66316192505535121"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>target_performance</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FCD184"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>hash!$O$4:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>hash!$Q$4:$Q$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>436</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>hash-single_core</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.6971088696064036E-4"/>
+                  <c:y val="8.2665122067316233E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1506850694141911E-2"/>
+                  <c:y val="4.0313125462376198E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.9847804965040917E-3"/>
+                  <c:y val="-2.3780101048912951E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.7321166040001206E-3"/>
+                  <c:y val="-3.5433414960056434E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.2100464063623018E-3"/>
+                  <c:y val="-3.252008648227056E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.6879762087244821E-3"/>
+                  <c:y val="-2.3780101048912951E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>hash!$O$4:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>hash!$P$4:$P$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>289</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>398</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>567</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="42074880"/>
+        <c:axId val="42076416"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="42074880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="8100000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="800" baseline="0"/>
+                  <a:t>network connections [n]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.81805196827046911"/>
+              <c:y val="0.84725418790968676"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="42076416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="42076416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="22225">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="42074880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln cmpd="sng">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3238,6 +3869,83 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.8067</cdr:x>
+      <cdr:y>0.36999</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.95739</cdr:x>
+      <cdr:y>0.43845</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6731047" y="1612905"/>
+          <a:ext cx="1257342" cy="298436"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="800"/>
+            <a:t>target performance = 436 </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4561,8 +5269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="O3:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4667,4 +5375,115 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="O2:T11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="15:20" x14ac:dyDescent="0.35">
+      <c r="Q2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="15:20" x14ac:dyDescent="0.35">
+      <c r="O3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>2</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+      <c r="T3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="15:20" x14ac:dyDescent="0.35">
+      <c r="O4">
+        <v>1000</v>
+      </c>
+      <c r="P4">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="5" spans="15:20" x14ac:dyDescent="0.35">
+      <c r="O5">
+        <v>10000</v>
+      </c>
+      <c r="P5">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="6" spans="15:20" x14ac:dyDescent="0.35">
+      <c r="O6">
+        <v>100000</v>
+      </c>
+      <c r="P6">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="7" spans="15:20" x14ac:dyDescent="0.35">
+      <c r="O7">
+        <v>500000</v>
+      </c>
+      <c r="P7">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="8" spans="15:20" x14ac:dyDescent="0.35">
+      <c r="O8">
+        <v>1000000</v>
+      </c>
+      <c r="P8">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="9" spans="15:20" x14ac:dyDescent="0.35">
+      <c r="O9">
+        <v>2000000</v>
+      </c>
+      <c r="P9">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="10" spans="15:20" x14ac:dyDescent="0.35">
+      <c r="O10">
+        <v>4000000</v>
+      </c>
+      <c r="P10">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="11" spans="15:20" x14ac:dyDescent="0.35">
+      <c r="O11">
+        <v>8000000</v>
+      </c>
+      <c r="P11">
+        <v>436</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="Q2:T2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
parallel chart and summary added
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -3291,7 +3291,7 @@
               <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>CPU: i5-4210U, 1 core</a:t>
+              <a:t>CPU: i5-4210U, 4 cores</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1100">
               <a:effectLst/>
@@ -3403,10 +3403,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>hash!$O$4:$O$11</c:f>
+              <c:f>parallel_hash!$O$4:$O$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3430,16 +3430,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>hash!$Q$4:$Q$11</c:f>
+              <c:f>parallel_hash!$P$4:$P$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>436</c:v>
                 </c:pt>
@@ -3462,6 +3465,9 @@
                   <c:v>436</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>436</c:v>
                 </c:pt>
               </c:numCache>
@@ -3470,144 +3476,22 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>hash-single_core</c:v>
+            <c:v>1_core</c:v>
           </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="40000"/>
-                  <a:lumOff val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="tx2">
-                    <a:lumMod val="60000"/>
-                    <a:lumOff val="40000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
+            <c:size val="3"/>
           </c:marker>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="6.6971088696064036E-4"/>
-                  <c:y val="8.2665122067316233E-3"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-1.1506850694141911E-2"/>
-                  <c:y val="4.0313125462376198E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-9.9847804965040917E-3"/>
-                  <c:y val="-2.3780101048912951E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-7.7321166040001206E-3"/>
-                  <c:y val="-3.5433414960056434E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-6.2100464063623018E-3"/>
-                  <c:y val="-3.252008648227056E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-4.6879762087244821E-3"/>
-                  <c:y val="-2.3780101048912951E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="600"/>
+                  <a:defRPr sz="500"/>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -3623,10 +3507,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>hash!$O$4:$O$11</c:f>
+              <c:f>parallel_hash!$O$4:$O$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3650,39 +3534,357 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>hash!$P$4:$P$11</c:f>
+              <c:f>parallel_hash!$Q$4:$Q$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>257</c:v>
+                  <c:v>334</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>260</c:v>
+                  <c:v>347</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>277</c:v>
+                  <c:v>363</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>289</c:v>
+                  <c:v>412</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>305</c:v>
+                  <c:v>431</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>335</c:v>
+                  <c:v>462</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>398</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>567</c:v>
+                  <c:v>678</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>963</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>2_core</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="500"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_hash!$O$4:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_hash!$R$4:$R$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>263</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>376</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>3_core</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="500"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_hash!$O$4:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_hash!$S$4:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>268</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>4_core</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="500"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_hash!$O$4:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_hash!$T$4:$T$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>194</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3705,7 +3907,7 @@
         <c:axId val="42074880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="8100000"/>
+          <c:max val="16100000.000000002"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3732,7 +3934,7 @@
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
               <c:x val="0.81805196827046911"/>
-              <c:y val="0.84725418790968676"/>
+              <c:y val="0.86911217245385308"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3767,6 +3969,7 @@
         <c:axId val="42076416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3883,8 +4086,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>419099</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3912,12 +4115,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.8067</cdr:x>
-      <cdr:y>0.36999</cdr:y>
+      <cdr:x>0.79148</cdr:x>
+      <cdr:y>0.57804</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.95739</cdr:x>
-      <cdr:y>0.43845</cdr:y>
+      <cdr:x>0.94217</cdr:x>
+      <cdr:y>0.61093</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -3926,8 +4129,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="6731047" y="1612905"/>
-          <a:ext cx="1257342" cy="298436"/>
+          <a:off x="6604023" y="3358542"/>
+          <a:ext cx="1257342" cy="191108"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5270,7 +5473,7 @@
   <dimension ref="O3:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:Q11"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5379,13 +5582,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="O2:T11"/>
+  <dimension ref="O2:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="15" max="15" width="11.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="15:20" x14ac:dyDescent="0.35">
       <c r="Q2" s="1" t="s">
@@ -5422,6 +5628,18 @@
       <c r="P4">
         <v>436</v>
       </c>
+      <c r="Q4">
+        <v>334</v>
+      </c>
+      <c r="R4">
+        <v>194</v>
+      </c>
+      <c r="S4">
+        <v>165</v>
+      </c>
+      <c r="T4">
+        <v>123</v>
+      </c>
     </row>
     <row r="5" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O5">
@@ -5430,6 +5648,18 @@
       <c r="P5">
         <v>436</v>
       </c>
+      <c r="Q5">
+        <v>347</v>
+      </c>
+      <c r="R5">
+        <v>197</v>
+      </c>
+      <c r="S5">
+        <v>154</v>
+      </c>
+      <c r="T5">
+        <v>99</v>
+      </c>
     </row>
     <row r="6" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O6">
@@ -5438,6 +5668,18 @@
       <c r="P6">
         <v>436</v>
       </c>
+      <c r="Q6">
+        <v>363</v>
+      </c>
+      <c r="R6">
+        <v>220</v>
+      </c>
+      <c r="S6">
+        <v>191</v>
+      </c>
+      <c r="T6">
+        <v>142</v>
+      </c>
     </row>
     <row r="7" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O7">
@@ -5446,6 +5688,18 @@
       <c r="P7">
         <v>436</v>
       </c>
+      <c r="Q7">
+        <v>412</v>
+      </c>
+      <c r="R7">
+        <v>262</v>
+      </c>
+      <c r="S7">
+        <v>197</v>
+      </c>
+      <c r="T7">
+        <v>162</v>
+      </c>
     </row>
     <row r="8" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O8">
@@ -5454,6 +5708,18 @@
       <c r="P8">
         <v>436</v>
       </c>
+      <c r="Q8">
+        <v>431</v>
+      </c>
+      <c r="R8">
+        <v>248</v>
+      </c>
+      <c r="S8">
+        <v>213</v>
+      </c>
+      <c r="T8">
+        <v>164</v>
+      </c>
     </row>
     <row r="9" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O9">
@@ -5462,6 +5728,18 @@
       <c r="P9">
         <v>436</v>
       </c>
+      <c r="Q9">
+        <v>462</v>
+      </c>
+      <c r="R9">
+        <v>263</v>
+      </c>
+      <c r="S9">
+        <v>197</v>
+      </c>
+      <c r="T9">
+        <v>166</v>
+      </c>
     </row>
     <row r="10" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O10">
@@ -5470,6 +5748,18 @@
       <c r="P10">
         <v>436</v>
       </c>
+      <c r="Q10">
+        <v>530</v>
+      </c>
+      <c r="R10">
+        <v>273</v>
+      </c>
+      <c r="S10">
+        <v>206</v>
+      </c>
+      <c r="T10">
+        <v>173</v>
+      </c>
     </row>
     <row r="11" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O11">
@@ -5477,6 +5767,38 @@
       </c>
       <c r="P11">
         <v>436</v>
+      </c>
+      <c r="Q11">
+        <v>678</v>
+      </c>
+      <c r="R11">
+        <v>308</v>
+      </c>
+      <c r="S11">
+        <v>228</v>
+      </c>
+      <c r="T11">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="15:20" x14ac:dyDescent="0.35">
+      <c r="O12">
+        <v>16000000</v>
+      </c>
+      <c r="P12">
+        <v>436</v>
+      </c>
+      <c r="Q12">
+        <v>963</v>
+      </c>
+      <c r="R12">
+        <v>376</v>
+      </c>
+      <c r="S12">
+        <v>268</v>
+      </c>
+      <c r="T12">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some additional charts in packet per second added
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="110" windowWidth="14360" windowHeight="4680" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="110" windowWidth="14360" windowHeight="4680" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Ideal NAT" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>chesums+timestamp</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>target</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>reg</t>
+  </si>
+  <si>
+    <t>rb</t>
   </si>
 </sst>
 </file>
@@ -319,11 +328,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="48049536"/>
-        <c:axId val="48055808"/>
+        <c:axId val="104566144"/>
+        <c:axId val="104589568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48049536"/>
+        <c:axId val="104566144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -341,7 +350,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="48055808"/>
+        <c:crossAx val="104589568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -349,7 +358,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48055808"/>
+        <c:axId val="104589568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -374,7 +383,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="48049536"/>
+        <c:crossAx val="104566144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1002,30 +1011,6 @@
                 <c:pt idx="19">
                   <c:v>3006</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>4444</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>5861</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7338</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>15852</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>22741</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>31142</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>40121</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>80154</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1040,11 +1025,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="71793664"/>
-        <c:axId val="48537984"/>
+        <c:axId val="121341440"/>
+        <c:axId val="121353728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71793664"/>
+        <c:axId val="121341440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2200"/>
@@ -1090,12 +1075,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="48537984"/>
+        <c:crossAx val="121353728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48537984"/>
+        <c:axId val="121353728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1120,7 +1105,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="71793664"/>
+        <c:crossAx val="121341440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1155,6 +1140,729 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr anchor="t" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0"/>
+              <a:t>Nat Performance - Linear Search </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>CPU: i5-4210U@2.4GHz, 1 core</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0"/>
+              <a:t>[Mpps]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.8471703696317515E-2"/>
+          <c:y val="1.2330720131214482E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.9429535280808154E-2"/>
+          <c:y val="0.23300827354297415"/>
+          <c:w val="0.8587591963900808"/>
+          <c:h val="0.66316192505535121"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>target_performance</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FCD184"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'linear search'!$O$6:$O$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'linear search'!$T$6:$T$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>linear search</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.4848095596555039E-3"/>
+                  <c:y val="1.3616484392473519E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.528949954931142E-3"/>
+                  <c:y val="-1.4222548474230234E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.5933083562013399E-4"/>
+                  <c:y val="-1.0351491933865149E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.1868313602549601E-2"/>
+                  <c:y val="-3.6665500570622303E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.0346243404911781E-2"/>
+                  <c:y val="-3.657121883799485E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:numFmt formatCode="0.00" sourceLinked="0"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'linear search'!$O$6:$O$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'linear search'!$R$6:$R$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>17.647058823529413</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.634146341463415</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.594202898550725</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.6021505376344081</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.8571428571428568</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.6872037914691944</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.8681541582150105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.2628774422735347</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.7735849056603774</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3707865168539324</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0341340075853349</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.8268551236749118</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.5641025641025643</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.416918429003021</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.2620169651272386</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.1071115013169446</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.9867549668874172</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.8764659890539483</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5374759769378603</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.79840319361277445</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="49101056"/>
+        <c:axId val="49111424"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="49101056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2200"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                  <a:t>nat table size [entries]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.44666684004684143"/>
+              <c:y val="0.95213401310997814"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="49111424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="49111424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="22225">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="49101056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln cmpd="sng">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1664,11 +2372,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="126960768"/>
-        <c:axId val="126962688"/>
+        <c:axId val="121398784"/>
+        <c:axId val="121423360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="126960768"/>
+        <c:axId val="121398784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1727,12 +2435,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126962688"/>
+        <c:crossAx val="121423360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="126962688"/>
+        <c:axId val="121423360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4000000"/>
@@ -1769,7 +2477,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126960768"/>
+        <c:crossAx val="121398784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1803,7 +2511,557 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr anchor="t" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0"/>
+              <a:t>Nat Performance - Binary tree-based NAT table </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>CPU: i5-4210U@2.4GHz, 1 core</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="800" b="1"/>
+              <a:t>[Kpps]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.4773071917577142E-2"/>
+          <c:y val="2.3984034042357966E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.9429535280808154E-2"/>
+          <c:y val="0.23300827354297415"/>
+          <c:w val="0.8587591963900808"/>
+          <c:h val="0.66316192505535121"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>binary tree</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1213822219084853E-2"/>
+                  <c:y val="-2.7170114296528665E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.8824173207273961E-2"/>
+                  <c:y val="-5.0948838969782716E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.404487518365204E-2"/>
+                  <c:y val="-2.2004805845008631E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.1868313602549601E-2"/>
+                  <c:y val="-3.6665500570622303E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.0346243404911781E-2"/>
+                  <c:y val="-3.657121883799485E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>tree_tree!$O$3:$O$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>tree_tree!$S$3:$S$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>228.09351834252044</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.970797454137028</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.63672367465967117</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>target_performance</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>tree_tree!$O$3:$O$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>tree_tree!$T$3:$T$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="78058240"/>
+        <c:axId val="78060160"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="78058240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="101000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="800" baseline="0"/>
+                  <a:t>nat table size [entries</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                  <a:t>]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.83175060004920953"/>
+              <c:y val="0.84142753095411504"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="78060160"/>
+        <c:crossesAt val="1.0000000000000002E-3"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="78060160"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="22225">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="78058240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln cmpd="sng">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2453,11 +3711,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69879296"/>
-        <c:axId val="69881216"/>
+        <c:axId val="121500032"/>
+        <c:axId val="121501952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69879296"/>
+        <c:axId val="121500032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2100000"/>
@@ -2517,12 +3775,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69881216"/>
+        <c:crossAx val="121501952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69881216"/>
+        <c:axId val="121501952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2558,7 +3816,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69879296"/>
+        <c:crossAx val="121500032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2592,7 +3850,813 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr anchor="t" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0"/>
+              <a:t>Nat Performance - Binary tree-based NAT table + 1D array </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>CPU: i5-4210U@2.4GHz, 1 core</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="800" b="1"/>
+              <a:t>[Mpps]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.9126195079782243E-2"/>
+          <c:y val="2.1070705564572093E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10551781607135943"/>
+          <c:y val="0.22426825561589944"/>
+          <c:w val="0.8587591963900808"/>
+          <c:h val="0.66316192505535121"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>target_performance</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FCD184"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>tree_array!$O$4:$O$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>tree_array!$V$4:$V$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>binary tree-array</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.5597385586762257E-2"/>
+                  <c:y val="2.137649035676804E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.4075315389124437E-2"/>
+                  <c:y val="2.4289818834553858E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.0163596179675713E-2"/>
+                  <c:y val="3.3029804267911522E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.9509104796210978E-2"/>
+                  <c:y val="3.5943132745697395E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6464964400935343E-2"/>
+                  <c:y val="2.7203147312339783E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6465084248982288E-2"/>
+                  <c:y val="3.0116475790125653E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>tree_array!$O$4:$O$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>tree_array!$T$4:$T$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.3829787234042552</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2173913043478262</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6474164133738602</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2079116835326587</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6404647983595353</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5686274509803921</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>red-black tree</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.8104730174706092E-3"/>
+                  <c:y val="-2.137649035676804E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.2884028198327765E-3"/>
+                  <c:y val="-1.263650492341043E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.332543215108428E-3"/>
+                  <c:y val="-2.428981883455391E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6464964400935343E-2"/>
+                  <c:y val="-2.7203147312339783E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.179221009266771E-2"/>
+                  <c:y val="-2.5746483073446846E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.0270259743076835E-2"/>
+                  <c:y val="-2.574671246938998E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>tree_array!$O$4:$O$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>tree_array!$U$4:$U$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.5934065934065931</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.6470588235294121</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8585209003215435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2813688212927756</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9543973941368078</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.791044776119403</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="110750336"/>
+        <c:axId val="110859008"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="110750336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2100000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="800" baseline="0"/>
+                  <a:t>nat table size [entries</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                  <a:t>]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.84088302123503644"/>
+              <c:y val="0.83851420247632924"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="110859008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="110859008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="22225">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="110750336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln cmpd="sng">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3077,11 +5141,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="70118784"/>
-        <c:axId val="70121344"/>
+        <c:axId val="121570048"/>
+        <c:axId val="121578240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70118784"/>
+        <c:axId val="121570048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8100000"/>
@@ -3138,12 +5202,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70121344"/>
+        <c:crossAx val="121578240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70121344"/>
+        <c:axId val="121578240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3179,7 +5243,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70118784"/>
+        <c:crossAx val="121570048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3213,7 +5277,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3900,11 +5964,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="42074880"/>
-        <c:axId val="42076416"/>
+        <c:axId val="121673984"/>
+        <c:axId val="121688448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42074880"/>
+        <c:axId val="121673984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16100000.000000002"/>
@@ -3961,12 +6025,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42076416"/>
+        <c:crossAx val="121688448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42076416"/>
+        <c:axId val="121688448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -4003,7 +6067,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42074880"/>
+        <c:crossAx val="121673984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4075,6 +6139,265 @@
 </file>
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.76332</cdr:x>
+      <cdr:y>0.32484</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.91401</cdr:x>
+      <cdr:y>0.3933</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6369097" y="1416055"/>
+          <a:ext cx="1257342" cy="298436"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="800"/>
+            <a:t>target performance = 5.5</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" baseline="0"/>
+            <a:t> Mpps</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.74962</cdr:x>
+      <cdr:y>0.7531</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.83409</cdr:x>
+      <cdr:y>0.81282</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6254762" y="3282952"/>
+          <a:ext cx="704810" cy="260336"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="800" b="1"/>
+            <a:t>regular binary tree</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.75191</cdr:x>
+      <cdr:y>0.65987</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.83638</cdr:x>
+      <cdr:y>0.71959</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="7" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6273821" y="2876553"/>
+          <a:ext cx="704809" cy="260336"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="800" b="1"/>
+            <a:t>red-black tree</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>603249</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>73025</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.8067</cdr:x>
+      <cdr:y>0.36999</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.95739</cdr:x>
+      <cdr:y>0.43845</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6731047" y="1612905"/>
+          <a:ext cx="1257342" cy="298436"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="800"/>
+            <a:t>target performance = 436 </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4111,7 +6434,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -4185,6 +6508,38 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4229,6 +6584,46 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.78082</cdr:x>
+      <cdr:y>0.65696</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.93151</cdr:x>
+      <cdr:y>0.72542</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6515072" y="2863855"/>
+          <a:ext cx="1257342" cy="298436"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="800"/>
+            <a:t>target performance = 5.5 Mpps </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4262,10 +6657,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>438149</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>136525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -4305,7 +6732,55 @@
 </c:userShapes>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.63775</cdr:x>
+      <cdr:y>0.22287</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.78844</cdr:x>
+      <cdr:y>0.29133</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5321309" y="971571"/>
+          <a:ext cx="1257342" cy="298436"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="800"/>
+            <a:t>target performance = 5500</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" baseline="0"/>
+            <a:t> Kpps</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4339,10 +6814,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>260349</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -4578,83 +7085,6 @@
           <a:r>
             <a:rPr lang="en-US" sz="800" b="1"/>
             <a:t>red-black tree</a:t>
-          </a:r>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>184150</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>603249</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>73025</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Диаграмма 4"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.8067</cdr:x>
-      <cdr:y>0.36999</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.95739</cdr:x>
-      <cdr:y>0.43845</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="4" name="TextBox 2"/>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="6731047" y="1612905"/>
-          <a:ext cx="1257342" cy="298436"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="800"/>
-            <a:t>target performance = 436 </a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -4950,39 +7380,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="P13:Q15"/>
+  <dimension ref="P13:R18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="16" max="16" width="28.54296875" customWidth="1"/>
+    <col min="18" max="18" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="13" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="16:18" x14ac:dyDescent="0.35">
       <c r="P13" t="s">
         <v>0</v>
       </c>
       <c r="Q13">
         <v>119</v>
       </c>
+      <c r="R13">
+        <f>Q13/P18</f>
+        <v>49.583333333333336</v>
+      </c>
     </row>
-    <row r="14" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="16:18" x14ac:dyDescent="0.35">
       <c r="P14" t="s">
         <v>1</v>
       </c>
       <c r="Q14">
         <v>82</v>
       </c>
+      <c r="R14">
+        <f>Q14/P18</f>
+        <v>34.166666666666671</v>
+      </c>
     </row>
-    <row r="15" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="16:18" x14ac:dyDescent="0.35">
       <c r="P15" t="s">
         <v>2</v>
       </c>
       <c r="Q15">
         <v>40</v>
+      </c>
+      <c r="R15">
+        <f>Q15/P18</f>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="17" spans="16:16" x14ac:dyDescent="0.35">
+      <c r="P17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="16:16" x14ac:dyDescent="0.35">
+      <c r="P18">
+        <v>2.4</v>
       </c>
     </row>
   </sheetData>
@@ -4994,18 +7447,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="O5:Q33"/>
+  <dimension ref="O5:T25"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5:Q27"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="N55" sqref="N55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="16" max="16" width="16.7265625" customWidth="1"/>
+    <col min="19" max="19" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O5" t="s">
         <v>3</v>
       </c>
@@ -5013,7 +7467,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O6">
         <v>10</v>
       </c>
@@ -5023,8 +7477,18 @@
       <c r="Q6">
         <v>436</v>
       </c>
+      <c r="R6">
+        <f>S6/P6</f>
+        <v>17.647058823529413</v>
+      </c>
+      <c r="S6">
+        <v>2400</v>
+      </c>
+      <c r="T6">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="7" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O7">
         <v>50</v>
       </c>
@@ -5034,8 +7498,18 @@
       <c r="Q7">
         <v>436</v>
       </c>
+      <c r="R7">
+        <f t="shared" ref="R7:R25" si="0">S7/P7</f>
+        <v>14.634146341463415</v>
+      </c>
+      <c r="S7">
+        <v>2400</v>
+      </c>
+      <c r="T7">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="8" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O8">
         <v>100</v>
       </c>
@@ -5045,8 +7519,18 @@
       <c r="Q8">
         <v>436</v>
       </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>11.594202898550725</v>
+      </c>
+      <c r="S8">
+        <v>2400</v>
+      </c>
+      <c r="T8">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="9" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O9">
         <v>200</v>
       </c>
@@ -5056,8 +7540,18 @@
       <c r="Q9">
         <v>436</v>
       </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>8.6021505376344081</v>
+      </c>
+      <c r="S9">
+        <v>2400</v>
+      </c>
+      <c r="T9">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="10" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O10">
         <v>300</v>
       </c>
@@ -5067,8 +7561,18 @@
       <c r="Q10">
         <v>436</v>
       </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>6.8571428571428568</v>
+      </c>
+      <c r="S10">
+        <v>2400</v>
+      </c>
+      <c r="T10">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="11" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O11">
         <v>400</v>
       </c>
@@ -5078,8 +7582,18 @@
       <c r="Q11">
         <v>436</v>
       </c>
+      <c r="R11">
+        <f t="shared" si="0"/>
+        <v>5.6872037914691944</v>
+      </c>
+      <c r="S11">
+        <v>2400</v>
+      </c>
+      <c r="T11">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="12" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O12">
         <v>500</v>
       </c>
@@ -5089,8 +7603,18 @@
       <c r="Q12">
         <v>436</v>
       </c>
+      <c r="R12">
+        <f t="shared" si="0"/>
+        <v>4.8681541582150105</v>
+      </c>
+      <c r="S12">
+        <v>2400</v>
+      </c>
+      <c r="T12">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="13" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O13">
         <v>600</v>
       </c>
@@ -5100,8 +7624,18 @@
       <c r="Q13">
         <v>436</v>
       </c>
+      <c r="R13">
+        <f t="shared" si="0"/>
+        <v>4.2628774422735347</v>
+      </c>
+      <c r="S13">
+        <v>2400</v>
+      </c>
+      <c r="T13">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="14" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O14">
         <v>700</v>
       </c>
@@ -5111,8 +7645,18 @@
       <c r="Q14">
         <v>436</v>
       </c>
+      <c r="R14">
+        <f t="shared" si="0"/>
+        <v>3.7735849056603774</v>
+      </c>
+      <c r="S14">
+        <v>2400</v>
+      </c>
+      <c r="T14">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="15" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O15">
         <v>800</v>
       </c>
@@ -5122,8 +7666,18 @@
       <c r="Q15">
         <v>436</v>
       </c>
+      <c r="R15">
+        <f t="shared" si="0"/>
+        <v>3.3707865168539324</v>
+      </c>
+      <c r="S15">
+        <v>2400</v>
+      </c>
+      <c r="T15">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="16" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O16">
         <v>900</v>
       </c>
@@ -5133,8 +7687,18 @@
       <c r="Q16">
         <v>436</v>
       </c>
+      <c r="R16">
+        <f t="shared" si="0"/>
+        <v>3.0341340075853349</v>
+      </c>
+      <c r="S16">
+        <v>2400</v>
+      </c>
+      <c r="T16">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="17" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O17">
         <v>1000</v>
       </c>
@@ -5144,8 +7708,18 @@
       <c r="Q17">
         <v>436</v>
       </c>
+      <c r="R17">
+        <f t="shared" si="0"/>
+        <v>2.8268551236749118</v>
+      </c>
+      <c r="S17">
+        <v>2400</v>
+      </c>
+      <c r="T17">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="18" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O18">
         <v>1100</v>
       </c>
@@ -5155,8 +7729,18 @@
       <c r="Q18">
         <v>436</v>
       </c>
+      <c r="R18">
+        <f t="shared" si="0"/>
+        <v>2.5641025641025643</v>
+      </c>
+      <c r="S18">
+        <v>2400</v>
+      </c>
+      <c r="T18">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="19" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O19">
         <v>1200</v>
       </c>
@@ -5166,8 +7750,18 @@
       <c r="Q19">
         <v>436</v>
       </c>
+      <c r="R19">
+        <f t="shared" si="0"/>
+        <v>2.416918429003021</v>
+      </c>
+      <c r="S19">
+        <v>2400</v>
+      </c>
+      <c r="T19">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="20" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O20">
         <v>1300</v>
       </c>
@@ -5177,8 +7771,18 @@
       <c r="Q20">
         <v>436</v>
       </c>
+      <c r="R20">
+        <f t="shared" si="0"/>
+        <v>2.2620169651272386</v>
+      </c>
+      <c r="S20">
+        <v>2400</v>
+      </c>
+      <c r="T20">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="21" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O21">
         <v>1400</v>
       </c>
@@ -5188,8 +7792,18 @@
       <c r="Q21">
         <v>436</v>
       </c>
+      <c r="R21">
+        <f t="shared" si="0"/>
+        <v>2.1071115013169446</v>
+      </c>
+      <c r="S21">
+        <v>2400</v>
+      </c>
+      <c r="T21">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="22" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O22">
         <v>1500</v>
       </c>
@@ -5199,8 +7813,18 @@
       <c r="Q22">
         <v>436</v>
       </c>
+      <c r="R22">
+        <f t="shared" si="0"/>
+        <v>1.9867549668874172</v>
+      </c>
+      <c r="S22">
+        <v>2400</v>
+      </c>
+      <c r="T22">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="23" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O23">
         <v>1600</v>
       </c>
@@ -5210,8 +7834,18 @@
       <c r="Q23">
         <v>436</v>
       </c>
+      <c r="R23">
+        <f t="shared" si="0"/>
+        <v>1.8764659890539483</v>
+      </c>
+      <c r="S23">
+        <v>2400</v>
+      </c>
+      <c r="T23">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="24" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O24">
         <v>2000</v>
       </c>
@@ -5221,8 +7855,18 @@
       <c r="Q24">
         <v>436</v>
       </c>
+      <c r="R24">
+        <f t="shared" si="0"/>
+        <v>1.5374759769378603</v>
+      </c>
+      <c r="S24">
+        <v>2400</v>
+      </c>
+      <c r="T24">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="25" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O25">
         <v>4000</v>
       </c>
@@ -5232,69 +7876,15 @@
       <c r="Q25">
         <v>436</v>
       </c>
-    </row>
-    <row r="26" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O26">
-        <v>6000</v>
-      </c>
-      <c r="P26">
-        <v>4444</v>
-      </c>
-    </row>
-    <row r="27" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O27">
-        <v>8000</v>
-      </c>
-      <c r="P27">
-        <v>5861</v>
-      </c>
-    </row>
-    <row r="28" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O28">
-        <v>10000</v>
-      </c>
-      <c r="P28">
-        <v>7338</v>
-      </c>
-    </row>
-    <row r="29" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O29">
-        <v>20000</v>
-      </c>
-      <c r="P29">
-        <v>15852</v>
-      </c>
-    </row>
-    <row r="30" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O30">
-        <v>30000</v>
-      </c>
-      <c r="P30">
-        <v>22741</v>
-      </c>
-    </row>
-    <row r="31" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O31">
-        <v>40000</v>
-      </c>
-      <c r="P31">
-        <v>31142</v>
-      </c>
-    </row>
-    <row r="32" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O32">
-        <v>50000</v>
-      </c>
-      <c r="P32">
-        <v>40121</v>
-      </c>
-    </row>
-    <row r="33" spans="15:16" x14ac:dyDescent="0.35">
-      <c r="O33">
-        <v>100000</v>
-      </c>
-      <c r="P33">
-        <v>80154</v>
+      <c r="R25">
+        <f t="shared" si="0"/>
+        <v>0.79840319361277445</v>
+      </c>
+      <c r="S25">
+        <v>2400</v>
+      </c>
+      <c r="T25">
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>
@@ -5305,15 +7895,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="O2:Q5"/>
+  <dimension ref="O2:T5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:Q5"/>
+    <sheetView topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="R42" sqref="R42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O2" t="s">
         <v>3</v>
       </c>
@@ -5321,7 +7911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O3">
         <v>1000</v>
       </c>
@@ -5331,8 +7921,18 @@
       <c r="Q3">
         <v>436</v>
       </c>
+      <c r="R3">
+        <v>2400000</v>
+      </c>
+      <c r="S3">
+        <f>R3/P3</f>
+        <v>228.09351834252044</v>
+      </c>
+      <c r="T3">
+        <v>5500</v>
+      </c>
     </row>
-    <row r="4" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O4">
         <v>10000</v>
       </c>
@@ -5342,8 +7942,18 @@
       <c r="Q4">
         <v>436</v>
       </c>
+      <c r="R4">
+        <v>2400000</v>
+      </c>
+      <c r="S4">
+        <f t="shared" ref="S4:S5" si="0">R4/P4</f>
+        <v>17.970797454137028</v>
+      </c>
+      <c r="T4">
+        <v>5500</v>
+      </c>
     </row>
-    <row r="5" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O5">
         <v>100000</v>
       </c>
@@ -5352,6 +7962,16 @@
       </c>
       <c r="Q5">
         <v>436</v>
+      </c>
+      <c r="R5">
+        <v>2400000</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>0.63672367465967117</v>
+      </c>
+      <c r="T5">
+        <v>5500</v>
       </c>
     </row>
   </sheetData>
@@ -5362,23 +7982,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="O3:R9"/>
+  <dimension ref="O3:V9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q16" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="15:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="15:22" x14ac:dyDescent="0.35">
       <c r="O3" t="s">
         <v>3</v>
       </c>
       <c r="P3" t="s">
         <v>4</v>
       </c>
+      <c r="T3" t="s">
+        <v>8</v>
+      </c>
+      <c r="U3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="15:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="15:22" x14ac:dyDescent="0.35">
       <c r="O4">
         <v>1000</v>
       </c>
@@ -5391,8 +8017,22 @@
       <c r="R4">
         <v>364</v>
       </c>
+      <c r="S4">
+        <v>2400</v>
+      </c>
+      <c r="T4">
+        <f>S4/P4</f>
+        <v>6.3829787234042552</v>
+      </c>
+      <c r="U4">
+        <f>S4/R4</f>
+        <v>6.5934065934065931</v>
+      </c>
+      <c r="V4">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="5" spans="15:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="15:22" x14ac:dyDescent="0.35">
       <c r="O5">
         <v>10000</v>
       </c>
@@ -5405,8 +8045,22 @@
       <c r="R5">
         <v>425</v>
       </c>
+      <c r="S5">
+        <v>2400</v>
+      </c>
+      <c r="T5">
+        <f t="shared" ref="T5:T9" si="0">S5/P5</f>
+        <v>5.2173913043478262</v>
+      </c>
+      <c r="U5">
+        <f t="shared" ref="U5:U9" si="1">S5/R5</f>
+        <v>5.6470588235294121</v>
+      </c>
+      <c r="V5">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="6" spans="15:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="15:22" x14ac:dyDescent="0.35">
       <c r="O6">
         <v>100000</v>
       </c>
@@ -5419,8 +8073,22 @@
       <c r="R6">
         <v>622</v>
       </c>
+      <c r="S6">
+        <v>2400</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>3.6474164133738602</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="1"/>
+        <v>3.8585209003215435</v>
+      </c>
+      <c r="V6">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="7" spans="15:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="15:22" x14ac:dyDescent="0.35">
       <c r="O7">
         <v>500000</v>
       </c>
@@ -5433,8 +8101,22 @@
       <c r="R7">
         <v>1052</v>
       </c>
+      <c r="S7">
+        <v>2400</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>2.2079116835326587</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="1"/>
+        <v>2.2813688212927756</v>
+      </c>
+      <c r="V7">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="8" spans="15:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="15:22" x14ac:dyDescent="0.35">
       <c r="O8">
         <v>1000000</v>
       </c>
@@ -5447,8 +8129,22 @@
       <c r="R8">
         <v>1228</v>
       </c>
+      <c r="S8">
+        <v>2400</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>1.6404647983595353</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="1"/>
+        <v>1.9543973941368078</v>
+      </c>
+      <c r="V8">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="9" spans="15:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="15:22" x14ac:dyDescent="0.35">
       <c r="O9">
         <v>2000000</v>
       </c>
@@ -5460,6 +8156,20 @@
       </c>
       <c r="R9">
         <v>1340</v>
+      </c>
+      <c r="S9">
+        <v>2400</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>1.5686274509803921</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="1"/>
+        <v>1.791044776119403</v>
+      </c>
+      <c r="V9">
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>
@@ -5584,7 +8294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="O2:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
charts in packet per second added
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="110" windowWidth="14360" windowHeight="4680" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="110" windowWidth="14360" windowHeight="4680" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Ideal NAT" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>chesums+timestamp</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>rb</t>
+  </si>
+  <si>
+    <t>frq</t>
   </si>
 </sst>
 </file>
@@ -416,6 +419,1706 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr anchor="t" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0"/>
+              <a:t>Nat Performance - Hash-based NAT table</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>CPU: i5-4210U, 4 cores</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="800" b="1"/>
+              <a:t>[cycles/packet]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.9126195079782243E-2"/>
+          <c:y val="2.1070705564572093E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.4863324687894712E-2"/>
+          <c:y val="0.23883489800482879"/>
+          <c:w val="0.8587591963900808"/>
+          <c:h val="0.66316192505535121"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>target_performance</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FCD184"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_hash!$O$4:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_hash!$P$4:$P$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>436</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>1_core</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="500"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_hash!$O$4:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_hash!$Q$4:$Q$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>363</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>431</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>462</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>678</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>963</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>2_core</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="500"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_hash!$O$4:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_hash!$R$4:$R$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>263</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>376</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>3_core</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="500"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_hash!$O$4:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_hash!$S$4:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>268</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>4_core</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="500"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_hash!$O$4:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_hash!$T$4:$T$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>194</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="121673984"/>
+        <c:axId val="121688448"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="121673984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="16100000.000000002"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="800" baseline="0"/>
+                  <a:t>network connections [n]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.81805196827046911"/>
+              <c:y val="0.86911217245385308"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="121688448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="121688448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="22225">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="121673984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln cmpd="sng">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr anchor="t" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0"/>
+              <a:t>Nat Performance - Hash-based NAT table</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>CPU: i5-4210U@2.4GHz, 4 cores</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="800" b="1"/>
+              <a:t>[Mpps]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.9126195079782243E-2"/>
+          <c:y val="2.1070705564572093E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.6385394885532535E-2"/>
+          <c:y val="0.24102061012865195"/>
+          <c:w val="0.8587591963900808"/>
+          <c:h val="0.66316192505535121"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>target_performance</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FCD184"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_hash!$O$4:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_hash!$Q$33:$Q$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>1_core</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_hash!$O$4:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_hash!$S$33:$S$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>7.1856287425149699</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9164265129682994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.6115702479338845</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.825242718446602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5684454756380513</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1948051948051948</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.5283018867924527</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5398230088495577</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.4922118380062304</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>2_core</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_hash!$O$4:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_hash!$T$33:$T$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>12.371134020618557</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.182741116751268</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.909090909090908</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.1603053435114496</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.67741935483871</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.1254752851711025</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.791208791208792</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.7922077922077921</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.3829787234042552</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>3_core</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_hash!$O$4:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_hash!$U$33:$U$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>14.545454545454545</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.584415584415584</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.565445026178011</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.182741116751268</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.267605633802816</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.182741116751268</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.650485436893204</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.526315789473685</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.9552238805970141</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>4_core</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_hash!$O$4:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_hash!$V$33:$V$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>19.512195121951219</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.242424242424242</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.901408450704224</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.814814814814815</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.634146341463415</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.457831325301205</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.872832369942197</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.371134020618557</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="55294208"/>
+        <c:axId val="55316864"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="55294208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="16200000.000000002"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="800" baseline="0"/>
+                  <a:t>network connections [n]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.81805196827046911"/>
+              <c:y val="0.86911217245385308"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="55316864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="55316864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="25"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="22225">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="55294208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln cmpd="sng">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
@@ -747,9 +2450,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>linear search</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln>
               <a:solidFill>
@@ -947,10 +2647,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'linear search'!$P$6:$P$33</c:f>
+              <c:f>'linear search'!$P$6:$P$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>136</c:v>
                 </c:pt>
@@ -1007,9 +2707,6 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>1561</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5355,7 +7052,7 @@
               <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>CPU: i5-4210U, 4 cores</a:t>
+              <a:t>CPU: i5-4210U@2.4 GHz, 1 core</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1100">
               <a:effectLst/>
@@ -5415,7 +7112,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="800" b="1"/>
-              <a:t>[cycles/packet]</a:t>
+              <a:t>[Mpps]</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5467,10 +7164,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>parallel_hash!$O$4:$O$12</c:f>
+              <c:f>hash!$O$4:$O$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -5494,45 +7191,39 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>8000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>parallel_hash!$P$4:$P$12</c:f>
+              <c:f>hash!$T$4:$T$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>436</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>436</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>436</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>436</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>436</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>436</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>436</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>436</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>436</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5540,22 +7231,145 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>1_core</c:v>
+            <c:v>hash-single_core</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="3"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.4313206477616099E-3"/>
+                  <c:y val="-2.383910477301486E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.8806127890162996E-3"/>
+                  <c:y val="2.3701213489260796E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.7928738536627547E-3"/>
+                  <c:y val="-1.21052459819629E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.1564206895557806E-3"/>
+                  <c:y val="-2.3758668190824991E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.159543242555113E-3"/>
+                  <c:y val="-2.6682652862829889E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.6879762087244821E-3"/>
+                  <c:y val="-2.3780101048912951E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="500"/>
+                  <a:defRPr sz="600"/>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -5571,10 +7385,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>parallel_hash!$O$4:$O$12</c:f>
+              <c:f>hash!$O$4:$O$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -5598,357 +7412,39 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>8000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>parallel_hash!$Q$4:$Q$12</c:f>
+              <c:f>hash!$R$4:$R$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>334</c:v>
+                  <c:v>9.3385214007782107</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>347</c:v>
+                  <c:v>9.2307692307692299</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>363</c:v>
+                  <c:v>8.6642599277978345</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>412</c:v>
+                  <c:v>8.3044982698961931</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>431</c:v>
+                  <c:v>7.8688524590163933</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>462</c:v>
+                  <c:v>7.1641791044776122</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>530</c:v>
+                  <c:v>6.0301507537688446</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>678</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>963</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>2_core</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="3"/>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="500"/>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>parallel_hash!$O$4:$O$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>parallel_hash!$R$4:$R$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>194</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>197</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>262</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>248</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>263</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>273</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>308</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>376</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>3_core</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="3"/>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="500"/>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>parallel_hash!$O$4:$O$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>parallel_hash!$S$4:$S$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>165</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>154</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>191</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>197</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>213</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>197</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>206</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>228</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>268</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:v>4_core</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="3"/>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="500"/>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="b"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>parallel_hash!$O$4:$O$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>parallel_hash!$T$4:$T$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>123</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>142</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>162</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>164</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>166</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>173</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>194</c:v>
+                  <c:v>4.2328042328042326</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5964,14 +7460,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121673984"/>
-        <c:axId val="121688448"/>
+        <c:axId val="115566080"/>
+        <c:axId val="115568000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121673984"/>
+        <c:axId val="115566080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="16100000.000000002"/>
+          <c:max val="8100000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -5998,7 +7494,7 @@
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
               <c:x val="0.81805196827046911"/>
-              <c:y val="0.86911217245385308"/>
+              <c:y val="0.84725418790968676"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -6025,15 +7521,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121688448"/>
+        <c:crossAx val="115568000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121688448"/>
+        <c:axId val="115568000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -6067,7 +7562,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121673984"/>
+        <c:crossAx val="115566080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6354,6 +7849,38 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>241301</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>156028</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>52614</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>95703</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6398,6 +7925,54 @@
 </file>
 
 <file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.77617</cdr:x>
+      <cdr:y>0.48407</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.92686</cdr:x>
+      <cdr:y>0.55253</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6457996" y="2078580"/>
+          <a:ext cx="1253788" cy="293965"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="800"/>
+            <a:t>target performance = 5.5</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" baseline="0"/>
+            <a:t> Mpps</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6431,10 +8006,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -6466,6 +8073,196 @@
           <a:r>
             <a:rPr lang="en-US" sz="800"/>
             <a:t>target performance = 436 </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.39136</cdr:x>
+      <cdr:y>0.7303</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.54205</cdr:x>
+      <cdr:y>0.76319</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3265487" y="4243225"/>
+          <a:ext cx="1257342" cy="191099"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>target performance = 5.5</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1" baseline="0"/>
+            <a:t> Mpps</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.8653</cdr:x>
+      <cdr:y>0.53333</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.92694</cdr:x>
+      <cdr:y>0.57377</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7219949" y="3098800"/>
+          <a:ext cx="514350" cy="234950"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="800" b="1"/>
+            <a:t>4 cores</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.8653</cdr:x>
+      <cdr:y>0.62623</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.92618</cdr:x>
+      <cdr:y>0.66885</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7219949" y="3638550"/>
+          <a:ext cx="508000" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="800" b="1">
+              <a:latin typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t>3 cores</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.8653</cdr:x>
+      <cdr:y>0.69617</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.92085</cdr:x>
+      <cdr:y>0.74208</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="12" name="TextBox 11"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7219949" y="4044950"/>
+          <a:ext cx="463550" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="800" b="1"/>
+            <a:t>2 cores</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.8653</cdr:x>
+      <cdr:y>0.79891</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.92542</cdr:x>
+      <cdr:y>0.84481</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="13" name="TextBox 12"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7219949" y="4641850"/>
+          <a:ext cx="501650" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="800" b="1"/>
+            <a:t>1 core</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -7447,10 +9244,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="O5:T25"/>
+  <dimension ref="O2:T25"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="N55" sqref="N55"/>
+    <sheetView topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7459,6 +9256,12 @@
     <col min="19" max="19" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="15:20" x14ac:dyDescent="0.35">
+      <c r="S2">
+        <f>2400/207</f>
+        <v>11.594202898550725</v>
+      </c>
+    </row>
     <row r="5" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O5" t="s">
         <v>3</v>
@@ -7984,7 +9787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="O3:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>
@@ -8180,15 +9983,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="O3:Q11"/>
+  <dimension ref="O3:T11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O3" t="s">
         <v>3</v>
       </c>
@@ -8196,7 +9999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O4">
         <v>1000</v>
       </c>
@@ -8206,8 +10009,18 @@
       <c r="Q4">
         <v>436</v>
       </c>
+      <c r="R4">
+        <f>S4/P4</f>
+        <v>9.3385214007782107</v>
+      </c>
+      <c r="S4">
+        <v>2400</v>
+      </c>
+      <c r="T4">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="5" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O5">
         <v>10000</v>
       </c>
@@ -8217,8 +10030,18 @@
       <c r="Q5">
         <v>436</v>
       </c>
+      <c r="R5">
+        <f t="shared" ref="R5:R11" si="0">S5/P5</f>
+        <v>9.2307692307692299</v>
+      </c>
+      <c r="S5">
+        <v>2400</v>
+      </c>
+      <c r="T5">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="6" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O6">
         <v>100000</v>
       </c>
@@ -8228,8 +10051,18 @@
       <c r="Q6">
         <v>436</v>
       </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>8.6642599277978345</v>
+      </c>
+      <c r="S6">
+        <v>2400</v>
+      </c>
+      <c r="T6">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="7" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O7">
         <v>500000</v>
       </c>
@@ -8239,8 +10072,18 @@
       <c r="Q7">
         <v>436</v>
       </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>8.3044982698961931</v>
+      </c>
+      <c r="S7">
+        <v>2400</v>
+      </c>
+      <c r="T7">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="8" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O8">
         <v>1000000</v>
       </c>
@@ -8250,8 +10093,18 @@
       <c r="Q8">
         <v>436</v>
       </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>7.8688524590163933</v>
+      </c>
+      <c r="S8">
+        <v>2400</v>
+      </c>
+      <c r="T8">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="9" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O9">
         <v>2000000</v>
       </c>
@@ -8261,8 +10114,18 @@
       <c r="Q9">
         <v>436</v>
       </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>7.1641791044776122</v>
+      </c>
+      <c r="S9">
+        <v>2400</v>
+      </c>
+      <c r="T9">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="10" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O10">
         <v>4000000</v>
       </c>
@@ -8272,8 +10135,18 @@
       <c r="Q10">
         <v>436</v>
       </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>6.0301507537688446</v>
+      </c>
+      <c r="S10">
+        <v>2400</v>
+      </c>
+      <c r="T10">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="11" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O11">
         <v>8000000</v>
       </c>
@@ -8282,6 +10155,16 @@
       </c>
       <c r="Q11">
         <v>436</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="0"/>
+        <v>4.2328042328042326</v>
+      </c>
+      <c r="S11">
+        <v>2400</v>
+      </c>
+      <c r="T11">
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>
@@ -8292,15 +10175,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="O2:T12"/>
+  <dimension ref="O2:Z41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R51" sqref="R51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="15" max="15" width="11.1796875" customWidth="1"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="15:20" x14ac:dyDescent="0.35">
@@ -8511,9 +10395,404 @@
         <v>194</v>
       </c>
     </row>
+    <row r="31" spans="16:26" x14ac:dyDescent="0.35">
+      <c r="W31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+    </row>
+    <row r="32" spans="16:26" x14ac:dyDescent="0.35">
+      <c r="P32" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>6</v>
+      </c>
+      <c r="R32" t="s">
+        <v>10</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="T32">
+        <v>2</v>
+      </c>
+      <c r="U32">
+        <v>3</v>
+      </c>
+      <c r="V32">
+        <v>4</v>
+      </c>
+      <c r="W32">
+        <v>1</v>
+      </c>
+      <c r="X32">
+        <v>2</v>
+      </c>
+      <c r="Y32">
+        <v>3</v>
+      </c>
+      <c r="Z32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="16:26" x14ac:dyDescent="0.35">
+      <c r="P33">
+        <v>1000</v>
+      </c>
+      <c r="Q33">
+        <v>5.5</v>
+      </c>
+      <c r="R33">
+        <v>2400</v>
+      </c>
+      <c r="S33">
+        <f>R33/W33</f>
+        <v>7.1856287425149699</v>
+      </c>
+      <c r="T33">
+        <f>R33/X33</f>
+        <v>12.371134020618557</v>
+      </c>
+      <c r="U33">
+        <f>R33/Y33</f>
+        <v>14.545454545454545</v>
+      </c>
+      <c r="V33">
+        <f>R33/Z33</f>
+        <v>19.512195121951219</v>
+      </c>
+      <c r="W33">
+        <v>334</v>
+      </c>
+      <c r="X33">
+        <v>194</v>
+      </c>
+      <c r="Y33">
+        <v>165</v>
+      </c>
+      <c r="Z33">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="16:26" x14ac:dyDescent="0.35">
+      <c r="P34">
+        <v>10000</v>
+      </c>
+      <c r="Q34">
+        <v>5.5</v>
+      </c>
+      <c r="R34">
+        <v>2400</v>
+      </c>
+      <c r="S34">
+        <f t="shared" ref="S34:S41" si="0">R34/W34</f>
+        <v>6.9164265129682994</v>
+      </c>
+      <c r="T34">
+        <f t="shared" ref="T34:T41" si="1">R34/X34</f>
+        <v>12.182741116751268</v>
+      </c>
+      <c r="U34">
+        <f t="shared" ref="U34:U41" si="2">R34/Y34</f>
+        <v>15.584415584415584</v>
+      </c>
+      <c r="V34">
+        <f t="shared" ref="V34:V41" si="3">R34/Z34</f>
+        <v>24.242424242424242</v>
+      </c>
+      <c r="W34">
+        <v>347</v>
+      </c>
+      <c r="X34">
+        <v>197</v>
+      </c>
+      <c r="Y34">
+        <v>154</v>
+      </c>
+      <c r="Z34">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="16:26" x14ac:dyDescent="0.35">
+      <c r="P35">
+        <v>100000</v>
+      </c>
+      <c r="Q35">
+        <v>5.5</v>
+      </c>
+      <c r="R35">
+        <v>2400</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="0"/>
+        <v>6.6115702479338845</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="1"/>
+        <v>10.909090909090908</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="2"/>
+        <v>12.565445026178011</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="3"/>
+        <v>16.901408450704224</v>
+      </c>
+      <c r="W35">
+        <v>363</v>
+      </c>
+      <c r="X35">
+        <v>220</v>
+      </c>
+      <c r="Y35">
+        <v>191</v>
+      </c>
+      <c r="Z35">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="16:26" x14ac:dyDescent="0.35">
+      <c r="P36">
+        <v>500000</v>
+      </c>
+      <c r="Q36">
+        <v>5.5</v>
+      </c>
+      <c r="R36">
+        <v>2400</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="0"/>
+        <v>5.825242718446602</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="1"/>
+        <v>9.1603053435114496</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="2"/>
+        <v>12.182741116751268</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="3"/>
+        <v>14.814814814814815</v>
+      </c>
+      <c r="W36">
+        <v>412</v>
+      </c>
+      <c r="X36">
+        <v>262</v>
+      </c>
+      <c r="Y36">
+        <v>197</v>
+      </c>
+      <c r="Z36">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="16:26" x14ac:dyDescent="0.35">
+      <c r="P37">
+        <v>1000000</v>
+      </c>
+      <c r="Q37">
+        <v>5.5</v>
+      </c>
+      <c r="R37">
+        <v>2400</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="0"/>
+        <v>5.5684454756380513</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="1"/>
+        <v>9.67741935483871</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="2"/>
+        <v>11.267605633802816</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="3"/>
+        <v>14.634146341463415</v>
+      </c>
+      <c r="W37">
+        <v>431</v>
+      </c>
+      <c r="X37">
+        <v>248</v>
+      </c>
+      <c r="Y37">
+        <v>213</v>
+      </c>
+      <c r="Z37">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="16:26" x14ac:dyDescent="0.35">
+      <c r="P38">
+        <v>2000000</v>
+      </c>
+      <c r="Q38">
+        <v>5.5</v>
+      </c>
+      <c r="R38">
+        <v>2400</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="0"/>
+        <v>5.1948051948051948</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="1"/>
+        <v>9.1254752851711025</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="2"/>
+        <v>12.182741116751268</v>
+      </c>
+      <c r="V38">
+        <f t="shared" si="3"/>
+        <v>14.457831325301205</v>
+      </c>
+      <c r="W38">
+        <v>462</v>
+      </c>
+      <c r="X38">
+        <v>263</v>
+      </c>
+      <c r="Y38">
+        <v>197</v>
+      </c>
+      <c r="Z38">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="16:26" x14ac:dyDescent="0.35">
+      <c r="P39">
+        <v>4000000</v>
+      </c>
+      <c r="Q39">
+        <v>5.5</v>
+      </c>
+      <c r="R39">
+        <v>2400</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="0"/>
+        <v>4.5283018867924527</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="1"/>
+        <v>8.791208791208792</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="2"/>
+        <v>11.650485436893204</v>
+      </c>
+      <c r="V39">
+        <f t="shared" si="3"/>
+        <v>13.872832369942197</v>
+      </c>
+      <c r="W39">
+        <v>530</v>
+      </c>
+      <c r="X39">
+        <v>273</v>
+      </c>
+      <c r="Y39">
+        <v>206</v>
+      </c>
+      <c r="Z39">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="16:26" x14ac:dyDescent="0.35">
+      <c r="P40">
+        <v>8000000</v>
+      </c>
+      <c r="Q40">
+        <v>5.5</v>
+      </c>
+      <c r="R40">
+        <v>2400</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="0"/>
+        <v>3.5398230088495577</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="1"/>
+        <v>7.7922077922077921</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="2"/>
+        <v>10.526315789473685</v>
+      </c>
+      <c r="V40">
+        <f t="shared" si="3"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="W40">
+        <v>678</v>
+      </c>
+      <c r="X40">
+        <v>308</v>
+      </c>
+      <c r="Y40">
+        <v>228</v>
+      </c>
+      <c r="Z40">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" spans="16:26" x14ac:dyDescent="0.35">
+      <c r="P41">
+        <v>16000000</v>
+      </c>
+      <c r="Q41">
+        <v>5.5</v>
+      </c>
+      <c r="R41">
+        <v>2400</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="0"/>
+        <v>2.4922118380062304</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="1"/>
+        <v>6.3829787234042552</v>
+      </c>
+      <c r="U41">
+        <f t="shared" si="2"/>
+        <v>8.9552238805970141</v>
+      </c>
+      <c r="V41">
+        <f t="shared" si="3"/>
+        <v>12.371134020618557</v>
+      </c>
+      <c r="W41">
+        <v>963</v>
+      </c>
+      <c r="X41">
+        <v>376</v>
+      </c>
+      <c r="Y41">
+        <v>268</v>
+      </c>
+      <c r="Z41">
+        <v>194</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="W31:Z31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
hash table size choosing charts added
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="110" windowWidth="14360" windowHeight="4680" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="110" windowWidth="14360" windowHeight="4680" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Ideal NAT" sheetId="3" r:id="rId1"/>
@@ -13,13 +13,15 @@
     <sheet name="tree_array" sheetId="6" r:id="rId4"/>
     <sheet name="hash" sheetId="8" r:id="rId5"/>
     <sheet name="parallel_hash" sheetId="9" r:id="rId6"/>
+    <sheet name="tree_hash" sheetId="10" r:id="rId7"/>
+    <sheet name="hash-size dependancy" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>chesums+timestamp</t>
   </si>
@@ -53,11 +55,23 @@
   <si>
     <t>frq</t>
   </si>
+  <si>
+    <t>hash</t>
+  </si>
+  <si>
+    <t>tree</t>
+  </si>
+  <si>
+    <t>opt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,11 +102,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,11 +346,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="104566144"/>
-        <c:axId val="104589568"/>
+        <c:axId val="118527104"/>
+        <c:axId val="118530048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="104566144"/>
+        <c:axId val="118527104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -353,7 +368,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="104589568"/>
+        <c:crossAx val="118530048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -361,7 +376,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104589568"/>
+        <c:axId val="118530048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -386,7 +401,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="104566144"/>
+        <c:crossAx val="118527104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1106,11 +1121,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121673984"/>
-        <c:axId val="121688448"/>
+        <c:axId val="119091968"/>
+        <c:axId val="119093888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121673984"/>
+        <c:axId val="119091968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16100000.000000002"/>
@@ -1167,12 +1182,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121688448"/>
+        <c:crossAx val="119093888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121688448"/>
+        <c:axId val="119093888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -1209,7 +1224,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121673984"/>
+        <c:crossAx val="119091968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1982,11 +1997,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="55294208"/>
-        <c:axId val="55316864"/>
+        <c:axId val="119344512"/>
+        <c:axId val="119367168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55294208"/>
+        <c:axId val="119344512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16200000.000000002"/>
@@ -2043,12 +2058,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55316864"/>
+        <c:crossAx val="119367168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55316864"/>
+        <c:axId val="119367168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -2085,9 +2100,1391 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55294208"/>
+        <c:crossAx val="119344512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln cmpd="sng">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr anchor="t" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0"/>
+              <a:t>Nat Performance - Hash-based NAT table</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>CPU: i5-4210U, 1 core</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="800" b="1"/>
+              <a:t>[cycles/packet]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.9126195079782243E-2"/>
+          <c:y val="2.1070705564572093E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.4863324687894712E-2"/>
+          <c:y val="0.23883489800482879"/>
+          <c:w val="0.8587591963900808"/>
+          <c:h val="0.66316192505535121"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>target</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>tree_hash!$N$5:$N$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>tree_hash!$R$5:$R$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>436</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tree_hash!$P$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>tree_hash!$N$5:$N$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>tree_hash!$P$5:$P$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>274</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>293</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>305</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="68150400"/>
+        <c:axId val="68152320"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="68150400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="16100000.000000002"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="800" baseline="0"/>
+                  <a:t>network connections [n]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.81805196827046911"/>
+              <c:y val="0.84725418790968676"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="68152320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="68152320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="22225">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="68150400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln cmpd="sng">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr anchor="t" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0"/>
+              <a:t>Hash table size performance dependance</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>CPU: i5-4210U, 1 core</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="800" b="1"/>
+              <a:t>[cycles/packet]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.1332558074368815E-2"/>
+          <c:y val="2.6986039230444805E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.4863324687894712E-2"/>
+          <c:y val="0.23883489800482879"/>
+          <c:w val="0.8587591963900808"/>
+          <c:h val="0.66316192505535121"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>hash</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0782918149466192E-2"/>
+                  <c:y val="3.0574567398260023E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.6654804270462634E-3"/>
+                  <c:y val="2.4659283118780073E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'hash-size dependancy'!$O$7:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'hash-size dependancy'!$N$7:$N$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1231</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>882</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>649</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>431</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>376</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>313</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="143147392"/>
+        <c:axId val="86799872"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="143147392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="800" baseline="0"/>
+                  <a:t>hash table size [2^n]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.81093451396867211"/>
+              <c:y val="0.84725408544698"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="86799872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="86799872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="22225">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="143147392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln cmpd="sng">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr anchor="t" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0"/>
+              <a:t>Hash table size performance dependance</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>CPU: i5-4210U, 1 core</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="800" b="1"/>
+              <a:t>[Mpps]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.1332558074368815E-2"/>
+          <c:y val="2.6986039230444805E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.4863324687894712E-2"/>
+          <c:y val="0.23883489800482879"/>
+          <c:w val="0.8587591963900808"/>
+          <c:h val="0.66316192505535121"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>hash</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0782918149466192E-2"/>
+                  <c:y val="3.0574567398260023E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.6654804270462634E-3"/>
+                  <c:y val="2.4659283118780073E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'hash-size dependancy'!$O$7:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'hash-size dependancy'!$Q$7:$Q$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.949634443541836</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7210884353741496</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6979969183359014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5684454756380513</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3829787234042552</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.6677316293929714</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="90899584"/>
+        <c:axId val="90901504"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="90899584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="800" baseline="0"/>
+                  <a:t>hash table size [2^n]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.81093451396867211"/>
+              <c:y val="0.84725408544698"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="90901504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="90901504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="22225">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="90899584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -2722,11 +4119,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121341440"/>
-        <c:axId val="121353728"/>
+        <c:axId val="118314496"/>
+        <c:axId val="118316032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121341440"/>
+        <c:axId val="118314496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2200"/>
@@ -2772,12 +4169,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="121353728"/>
+        <c:crossAx val="118316032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121353728"/>
+        <c:axId val="118316032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2802,7 +4199,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="121341440"/>
+        <c:crossAx val="118314496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3445,11 +4842,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="49101056"/>
-        <c:axId val="49111424"/>
+        <c:axId val="118561408"/>
+        <c:axId val="118581888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49101056"/>
+        <c:axId val="118561408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2200"/>
@@ -3495,12 +4892,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="49111424"/>
+        <c:crossAx val="118581888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49111424"/>
+        <c:axId val="118581888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3525,7 +4922,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="49101056"/>
+        <c:crossAx val="118561408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4069,11 +5466,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121398784"/>
-        <c:axId val="121423360"/>
+        <c:axId val="118657024"/>
+        <c:axId val="118677504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121398784"/>
+        <c:axId val="118657024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -4132,12 +5529,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121423360"/>
+        <c:crossAx val="118677504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121423360"/>
+        <c:axId val="118677504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4000000"/>
@@ -4174,7 +5571,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121398784"/>
+        <c:crossAx val="118657024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4619,11 +6016,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="78058240"/>
-        <c:axId val="78060160"/>
+        <c:axId val="118703232"/>
+        <c:axId val="118705152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="78058240"/>
+        <c:axId val="118703232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="101000"/>
@@ -4683,12 +6080,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78060160"/>
+        <c:crossAx val="118705152"/>
         <c:crossesAt val="1.0000000000000002E-3"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78060160"/>
+        <c:axId val="118705152"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4724,7 +6121,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78058240"/>
+        <c:crossAx val="118703232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5408,11 +6805,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121500032"/>
-        <c:axId val="121501952"/>
+        <c:axId val="119166848"/>
+        <c:axId val="119189504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121500032"/>
+        <c:axId val="119166848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2100000"/>
@@ -5472,12 +6869,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121501952"/>
+        <c:crossAx val="119189504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121501952"/>
+        <c:axId val="119189504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -5513,7 +6910,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121500032"/>
+        <c:crossAx val="119166848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6214,11 +7611,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="110750336"/>
-        <c:axId val="110859008"/>
+        <c:axId val="119249152"/>
+        <c:axId val="119267712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110750336"/>
+        <c:axId val="119249152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2100000"/>
@@ -6278,12 +7675,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110859008"/>
+        <c:crossAx val="119267712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110859008"/>
+        <c:axId val="119267712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6319,7 +7716,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110750336"/>
+        <c:crossAx val="119249152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6838,11 +8235,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121570048"/>
-        <c:axId val="121578240"/>
+        <c:axId val="118931840"/>
+        <c:axId val="118976896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121570048"/>
+        <c:axId val="118931840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8100000"/>
@@ -6899,12 +8296,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121578240"/>
+        <c:crossAx val="118976896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121578240"/>
+        <c:axId val="118976896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6940,7 +8337,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121570048"/>
+        <c:crossAx val="118931840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7460,11 +8857,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115566080"/>
-        <c:axId val="115568000"/>
+        <c:axId val="118992256"/>
+        <c:axId val="119008640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115566080"/>
+        <c:axId val="118992256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8100000"/>
@@ -7521,12 +8918,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115568000"/>
+        <c:crossAx val="119008640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115568000"/>
+        <c:axId val="119008640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -7562,7 +8959,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115566080"/>
+        <c:crossAx val="118992256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8271,6 +9668,309 @@
 </c:userShapes>
 </file>
 
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>431801</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>58511</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.78624</cdr:x>
+      <cdr:y>0.2783</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.93693</cdr:x>
+      <cdr:y>0.34676</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5611691" y="1195023"/>
+          <a:ext cx="1075534" cy="293964"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="800"/>
+            <a:t>target performance = 436 </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>442686</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>58511</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>297963</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>117232</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>313906</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>174924</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5167095" y="1039779"/>
+          <a:ext cx="15943" cy="2825334"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>31751</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>12701</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4057650" y="1136651"/>
+          <a:ext cx="1238250" cy="165100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0"/>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>target</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1" baseline="0"/>
+            <a:t> NAT table size</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t> = 65.5M </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>26761</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -8338,6 +10038,433 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.09452</cdr:x>
+      <cdr:y>0.69525</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.95217</cdr:x>
+      <cdr:y>0.69525</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="5" name="Straight Connector 4"/>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="675673" y="3008818"/>
+          <a:ext cx="6130550" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050"/>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.72509</cdr:x>
+      <cdr:y>0.69652</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.95285</cdr:x>
+      <cdr:y>0.8984</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Rectangle 1"/>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5167605" y="2996608"/>
+          <a:ext cx="1623199" cy="868505"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:srgbClr val="FCD184">
+            <a:alpha val="22000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+          <a:noFill/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.09675</cdr:x>
+      <cdr:y>0.65948</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.24744</cdr:x>
+      <cdr:y>0.72794</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="689610" y="2828475"/>
+          <a:ext cx="1074083" cy="293621"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>target performance = 436 </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.09452</cdr:x>
+      <cdr:y>0.49857</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.95217</cdr:x>
+      <cdr:y>0.49857</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="5" name="Straight Connector 4"/>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="674627" y="2140826"/>
+          <a:ext cx="6121391" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050"/>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.71823</cdr:x>
+      <cdr:y>0.24</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.95483</cdr:x>
+      <cdr:y>0.49772</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Rectangle 1"/>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5121710" y="1033895"/>
+          <a:ext cx="1687221" cy="1110207"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:srgbClr val="FCD184">
+            <a:alpha val="22000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+          <a:noFill/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.09764</cdr:x>
+      <cdr:y>0.4628</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.24833</cdr:x>
+      <cdr:y>0.53126</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="696893" y="1987231"/>
+          <a:ext cx="1075535" cy="293965"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>target performance = 5.5</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1" baseline="0"/>
+            <a:t> Mpps</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.71804</cdr:x>
+      <cdr:y>0.24067</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.71845</cdr:x>
+      <cdr:y>0.89864</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="6" name="Straight Connector 5"/>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1" flipV="1">
+          <a:off x="5120409" y="1036783"/>
+          <a:ext cx="2886" cy="2834408"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050"/>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.56317</cdr:x>
+      <cdr:y>0.25879</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.73665</cdr:x>
+      <cdr:y>0.29724</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="11" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4019550" y="1111250"/>
+          <a:ext cx="1238250" cy="165100"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>target</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1" baseline="0"/>
+            <a:t> NAT table size</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t> = 65.5M </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9985,7 +12112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="O3:T11"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
@@ -10177,7 +12304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="O2:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="R51" sqref="R51"/>
     </sheetView>
   </sheetViews>
@@ -10797,4 +12924,374 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="N4:R11"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="4" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="O4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="N5">
+        <v>100000</v>
+      </c>
+      <c r="O5">
+        <v>264</v>
+      </c>
+      <c r="P5">
+        <v>259</v>
+      </c>
+      <c r="Q5">
+        <v>258</v>
+      </c>
+      <c r="R5">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="6" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="N6">
+        <v>1000000</v>
+      </c>
+      <c r="O6">
+        <v>295</v>
+      </c>
+      <c r="P6">
+        <v>284</v>
+      </c>
+      <c r="Q6">
+        <v>271</v>
+      </c>
+      <c r="R6">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="7" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="N7">
+        <v>2000000</v>
+      </c>
+      <c r="O7">
+        <v>284</v>
+      </c>
+      <c r="P7">
+        <v>274</v>
+      </c>
+      <c r="Q7">
+        <v>285</v>
+      </c>
+      <c r="R7">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="8" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="N8">
+        <v>4000000</v>
+      </c>
+      <c r="O8">
+        <v>289</v>
+      </c>
+      <c r="P8">
+        <v>271</v>
+      </c>
+      <c r="Q8">
+        <v>281</v>
+      </c>
+      <c r="R8">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="9" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="N9">
+        <v>8000000</v>
+      </c>
+      <c r="O9">
+        <v>275</v>
+      </c>
+      <c r="P9">
+        <v>271</v>
+      </c>
+      <c r="Q9">
+        <v>284</v>
+      </c>
+      <c r="R9">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="10" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="N10">
+        <v>16000000</v>
+      </c>
+      <c r="O10">
+        <v>284</v>
+      </c>
+      <c r="P10">
+        <v>293</v>
+      </c>
+      <c r="Q10">
+        <v>286</v>
+      </c>
+      <c r="R10">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="11" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="N11">
+        <v>32000000</v>
+      </c>
+      <c r="O11">
+        <v>321</v>
+      </c>
+      <c r="P11">
+        <v>305</v>
+      </c>
+      <c r="R11">
+        <v>436</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="M5:R16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="13" max="13" width="11.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="13:18" x14ac:dyDescent="0.35">
+      <c r="M5">
+        <f>2^O5</f>
+        <v>1048576</v>
+      </c>
+      <c r="N5">
+        <v>3542</v>
+      </c>
+      <c r="O5">
+        <v>20</v>
+      </c>
+      <c r="P5">
+        <v>436</v>
+      </c>
+      <c r="Q5" s="2">
+        <f>R5/N5</f>
+        <v>0.67758328627893849</v>
+      </c>
+      <c r="R5">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="6" spans="13:18" x14ac:dyDescent="0.35">
+      <c r="M6">
+        <f t="shared" ref="M6:M12" si="0">2^O6</f>
+        <v>2097152</v>
+      </c>
+      <c r="N6">
+        <v>2459</v>
+      </c>
+      <c r="O6">
+        <v>21</v>
+      </c>
+      <c r="P6">
+        <v>436</v>
+      </c>
+      <c r="Q6" s="2">
+        <f t="shared" ref="Q6:Q12" si="1">R6/N6</f>
+        <v>0.97600650671004474</v>
+      </c>
+      <c r="R6">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="7" spans="13:18" x14ac:dyDescent="0.35">
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>4194304</v>
+      </c>
+      <c r="N7">
+        <v>1231</v>
+      </c>
+      <c r="O7">
+        <v>22</v>
+      </c>
+      <c r="P7">
+        <v>436</v>
+      </c>
+      <c r="Q7" s="2">
+        <f t="shared" si="1"/>
+        <v>1.949634443541836</v>
+      </c>
+      <c r="R7">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="8" spans="13:18" x14ac:dyDescent="0.35">
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>8388608</v>
+      </c>
+      <c r="N8">
+        <v>882</v>
+      </c>
+      <c r="O8">
+        <v>23</v>
+      </c>
+      <c r="P8">
+        <v>436</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" si="1"/>
+        <v>2.7210884353741496</v>
+      </c>
+      <c r="R8">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="9" spans="13:18" x14ac:dyDescent="0.35">
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>16777216</v>
+      </c>
+      <c r="N9">
+        <v>649</v>
+      </c>
+      <c r="O9">
+        <v>24</v>
+      </c>
+      <c r="P9">
+        <v>436</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="1"/>
+        <v>3.6979969183359014</v>
+      </c>
+      <c r="R9">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="10" spans="13:18" x14ac:dyDescent="0.35">
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>33554432</v>
+      </c>
+      <c r="N10">
+        <v>431</v>
+      </c>
+      <c r="O10">
+        <v>25</v>
+      </c>
+      <c r="P10">
+        <v>436</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" si="1"/>
+        <v>5.5684454756380513</v>
+      </c>
+      <c r="R10">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="11" spans="13:18" x14ac:dyDescent="0.35">
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>67108864</v>
+      </c>
+      <c r="N11">
+        <v>376</v>
+      </c>
+      <c r="O11">
+        <v>26</v>
+      </c>
+      <c r="P11">
+        <v>436</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="1"/>
+        <v>6.3829787234042552</v>
+      </c>
+      <c r="R11">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="12" spans="13:18" x14ac:dyDescent="0.35">
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>134217728</v>
+      </c>
+      <c r="N12">
+        <v>313</v>
+      </c>
+      <c r="O12">
+        <v>27</v>
+      </c>
+      <c r="P12">
+        <v>436</v>
+      </c>
+      <c r="Q12" s="2">
+        <f t="shared" si="1"/>
+        <v>7.6677316293929714</v>
+      </c>
+      <c r="R12">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="16" spans="13:18" x14ac:dyDescent="0.35">
+      <c r="M16">
+        <f>LOG(65500000,2)</f>
+        <v>25.964991570861624</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries theme="4" tint="-0.499984740745262"/>
+          <x14:colorNegative theme="5"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="4" tint="-0.499984740745262"/>
+          <x14:colorFirst theme="4" tint="0.39997558519241921"/>
+          <x14:colorLast theme="4" tint="0.39997558519241921"/>
+          <x14:colorHigh theme="4"/>
+          <x14:colorLow theme="4"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'hash-size dependancy'!P5:P10</xm:f>
+              <xm:sqref>M17</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
hash table comparision charts and description added
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="110" windowWidth="14360" windowHeight="4680" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="360" yWindow="110" windowWidth="14360" windowHeight="4680" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Ideal NAT" sheetId="3" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="parallel_hash" sheetId="9" r:id="rId6"/>
     <sheet name="tree_hash" sheetId="10" r:id="rId7"/>
     <sheet name="hash-size dependancy" sheetId="11" r:id="rId8"/>
+    <sheet name="hash_table comparison" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>chesums+timestamp</t>
   </si>
@@ -64,6 +65,9 @@
   <si>
     <t>opt</t>
   </si>
+  <si>
+    <t>opt2</t>
+  </si>
 </sst>
 </file>
 
@@ -102,12 +106,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,11 +351,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="118527104"/>
-        <c:axId val="118530048"/>
+        <c:axId val="120612352"/>
+        <c:axId val="120615296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="118527104"/>
+        <c:axId val="120612352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -368,7 +373,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="118530048"/>
+        <c:crossAx val="120615296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -376,7 +381,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118530048"/>
+        <c:axId val="120615296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -401,7 +406,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="118527104"/>
+        <c:crossAx val="120612352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1121,11 +1126,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119091968"/>
-        <c:axId val="119093888"/>
+        <c:axId val="54240384"/>
+        <c:axId val="54242304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119091968"/>
+        <c:axId val="54240384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16100000.000000002"/>
@@ -1182,12 +1187,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119093888"/>
+        <c:crossAx val="54242304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119093888"/>
+        <c:axId val="54242304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -1224,7 +1229,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119091968"/>
+        <c:crossAx val="54240384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1997,11 +2002,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119344512"/>
-        <c:axId val="119367168"/>
+        <c:axId val="54378496"/>
+        <c:axId val="54380416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119344512"/>
+        <c:axId val="54378496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16200000.000000002"/>
@@ -2058,12 +2063,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119367168"/>
+        <c:crossAx val="54380416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119367168"/>
+        <c:axId val="54380416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -2100,7 +2105,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119344512"/>
+        <c:crossAx val="54378496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2500,11 +2505,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="68150400"/>
-        <c:axId val="68152320"/>
+        <c:axId val="54270976"/>
+        <c:axId val="54299648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68150400"/>
+        <c:axId val="54270976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16100000.000000002"/>
@@ -2561,12 +2566,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68152320"/>
+        <c:crossAx val="54299648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68152320"/>
+        <c:axId val="54299648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2602,7 +2607,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68150400"/>
+        <c:crossAx val="54270976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2939,11 +2944,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143147392"/>
-        <c:axId val="86799872"/>
+        <c:axId val="54430720"/>
+        <c:axId val="54454528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143147392"/>
+        <c:axId val="54430720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2998,7 +3003,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86799872"/>
+        <c:crossAx val="54454528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3006,7 +3011,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86799872"/>
+        <c:axId val="54454528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3042,7 +3047,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143147392"/>
+        <c:crossAx val="54430720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3379,11 +3384,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="90899584"/>
-        <c:axId val="90901504"/>
+        <c:axId val="53735808"/>
+        <c:axId val="53736960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="90899584"/>
+        <c:axId val="53735808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3438,7 +3443,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90901504"/>
+        <c:crossAx val="53736960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3446,7 +3451,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90901504"/>
+        <c:axId val="53736960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3482,9 +3487,2076 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90899584"/>
+        <c:crossAx val="53735808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln cmpd="sng">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr anchor="t" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0"/>
+              <a:t>Hash table performance comparison</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>CPU: i5-4210U, 1 core</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="800" b="1"/>
+              <a:t>[cycles/packet]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.1332558074368815E-2"/>
+          <c:y val="2.6986039230444805E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.4863324687894712E-2"/>
+          <c:y val="0.23883489800482879"/>
+          <c:w val="0.8587591963900808"/>
+          <c:h val="0.66316192505535121"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>hash</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.1992090970533964E-3"/>
+                  <c:y val="2.7600833521131133E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'hash_table comparison'!$N$6:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'hash_table comparison'!$O$6:$O$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>357</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>398</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>518</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>743</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>881</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'hash_table comparison'!$Q$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>opt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.1308801911701241E-2"/>
+                  <c:y val="1.8641430965953901E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.9541902914047737E-2"/>
+                  <c:y val="2.1582888775605557E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.4067109328197176E-3"/>
+                  <c:y val="-1.0773147130561584E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.8729129375127127E-3"/>
+                  <c:y val="9.9268410804460925E-4"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'hash_table comparison'!$N$6:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'hash_table comparison'!$Q$6:$Q$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>314</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>438</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>591</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'hash_table comparison'!$S$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>opt2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.1308801911701241E-2"/>
+                  <c:y val="-1.3714604940213133E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.9405089281267228E-3"/>
+                  <c:y val="-1.665606274986468E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0601393985921016E-4"/>
+                  <c:y val="-1.9487737016069392E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'hash_table comparison'!$N$6:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'hash_table comparison'!$S$6:$S$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>261</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>314</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>369</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>668</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'hash_table comparison'!$U$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.8729129375127127E-3"/>
+                  <c:y val="9.9268410804460925E-4"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.1308801911701241E-2"/>
+                  <c:y val="-1.9597520559516229E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0601393985921016E-4"/>
+                  <c:y val="-4.8902315112584879E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'hash_table comparison'!$N$6:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'hash_table comparison'!$U$6:$U$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>269</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>397</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="58435456"/>
+        <c:axId val="57335168"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="58435456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="800" baseline="0"/>
+                  <a:t>connections number [n]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.8074007747086912"/>
+              <c:y val="0.85607840675821933"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="57335168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="57335168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="900"/>
+          <c:min val="200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="22225">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="58435456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln cmpd="sng">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr anchor="t" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0"/>
+              <a:t>Hash table performance comparison</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>CPU: i5-4210U, 1 core</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="800" b="1"/>
+              <a:t>[cycles/packet]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.1332558074368815E-2"/>
+          <c:y val="2.6986039230444805E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.4863324687894712E-2"/>
+          <c:y val="0.23883489800482879"/>
+          <c:w val="0.8587591963900808"/>
+          <c:h val="0.66316192505535121"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>hash</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.488477607001905E-2"/>
+                  <c:y val="2.7600835224561183E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.2279550375664058E-4"/>
+                  <c:y val="-1.917588806423003E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'hash_table comparison'!$N$6:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'hash_table comparison'!$P$6:$P$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>7.717041800643087</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2072072072072073</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.4074074074074074</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.7226890756302522</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.9767441860465116</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0301507537688446</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.6332046332046328</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2301480484522207</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.7241770715096481</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'hash_table comparison'!$Q$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>opt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.6614475359130887E-2"/>
+                  <c:y val="-3.3457754018982627E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.3935257359786224E-3"/>
+                  <c:y val="-1.6044251768881041E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.1323859837680374E-2"/>
+                  <c:y val="-2.5244985986149784E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.8729129375127127E-3"/>
+                  <c:y val="9.9268410804460925E-4"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'hash_table comparison'!$N$6:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'hash_table comparison'!$R$6:$R$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>9.3385214007782107</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.3023255813953494</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.9887640449438209</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.695652173913043</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.6330935251798557</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.6433121019108281</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.8571428571428568</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.4794520547945202</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0609137055837561</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'hash_table comparison'!$S$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>opt2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.9289581127575332E-3"/>
+                  <c:y val="-7.9260641204867491E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.9405089281267228E-3"/>
+                  <c:y val="-1.665606274986468E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.8745255720742618E-3"/>
+                  <c:y val="3.8399636082029225E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'hash_table comparison'!$N$6:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'hash_table comparison'!$T$6:$T$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>9.3023255813953494</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.1954022988505741</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.9552238805970141</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.6330935251798557</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.4507042253521121</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.6433121019108281</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5040650406504064</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.1282051282051286</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5928143712574849</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'hash_table comparison'!$U$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.0169682093775855E-2"/>
+                  <c:y val="2.9936628863380801E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.5457233982317517E-2"/>
+                  <c:y val="1.8029528223926238E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.8585342438264662E-2"/>
+                  <c:y val="9.659961867012231E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.8745255720742618E-3"/>
+                  <c:y val="8.9862760443611633E-4"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'hash_table comparison'!$N$6:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'hash_table comparison'!$V$6:$V$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>9.2664092664092657</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.2664092664092657</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.921933085501859</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.5409252669039137</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.2191780821917817</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.2727272727272725</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0453400503778338</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.8780487804878048</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="83141376"/>
+        <c:axId val="83143296"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="83141376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="800" baseline="0"/>
+                  <a:t>connections number [n]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.8074007747086912"/>
+              <c:y val="0.85607840675821933"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="83143296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="83143296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="22225">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="83141376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -4119,11 +6191,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118314496"/>
-        <c:axId val="118316032"/>
+        <c:axId val="120571776"/>
+        <c:axId val="120573312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118314496"/>
+        <c:axId val="120571776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2200"/>
@@ -4169,12 +6241,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="118316032"/>
+        <c:crossAx val="120573312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118316032"/>
+        <c:axId val="120573312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4199,7 +6271,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="118314496"/>
+        <c:crossAx val="120571776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4842,11 +6914,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118561408"/>
-        <c:axId val="118581888"/>
+        <c:axId val="53300224"/>
+        <c:axId val="53320704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118561408"/>
+        <c:axId val="53300224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2200"/>
@@ -4892,12 +6964,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="118581888"/>
+        <c:crossAx val="53320704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118581888"/>
+        <c:axId val="53320704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4922,7 +6994,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="118561408"/>
+        <c:crossAx val="53300224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5466,11 +7538,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118657024"/>
-        <c:axId val="118677504"/>
+        <c:axId val="53619328"/>
+        <c:axId val="53648000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118657024"/>
+        <c:axId val="53619328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -5529,12 +7601,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118677504"/>
+        <c:crossAx val="53648000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118677504"/>
+        <c:axId val="53648000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4000000"/>
@@ -5571,7 +7643,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118657024"/>
+        <c:crossAx val="53619328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6016,11 +8088,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118703232"/>
-        <c:axId val="118705152"/>
+        <c:axId val="53690368"/>
+        <c:axId val="53692288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118703232"/>
+        <c:axId val="53690368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="101000"/>
@@ -6080,12 +8152,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118705152"/>
+        <c:crossAx val="53692288"/>
         <c:crossesAt val="1.0000000000000002E-3"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118705152"/>
+        <c:axId val="53692288"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6121,7 +8193,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118703232"/>
+        <c:crossAx val="53690368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6805,11 +8877,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119166848"/>
-        <c:axId val="119189504"/>
+        <c:axId val="53795072"/>
+        <c:axId val="53813632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119166848"/>
+        <c:axId val="53795072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2100000"/>
@@ -6869,12 +8941,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119189504"/>
+        <c:crossAx val="53813632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119189504"/>
+        <c:axId val="53813632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6910,7 +8982,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119166848"/>
+        <c:crossAx val="53795072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7611,11 +9683,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119249152"/>
-        <c:axId val="119267712"/>
+        <c:axId val="53866880"/>
+        <c:axId val="53868800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119249152"/>
+        <c:axId val="53866880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2100000"/>
@@ -7675,12 +9747,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119267712"/>
+        <c:crossAx val="53868800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119267712"/>
+        <c:axId val="53868800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -7716,7 +9788,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119249152"/>
+        <c:crossAx val="53866880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8235,11 +10307,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118931840"/>
-        <c:axId val="118976896"/>
+        <c:axId val="53482624"/>
+        <c:axId val="53484544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118931840"/>
+        <c:axId val="53482624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8100000"/>
@@ -8296,12 +10368,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118976896"/>
+        <c:crossAx val="53484544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118976896"/>
+        <c:axId val="53484544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -8337,7 +10409,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118931840"/>
+        <c:crossAx val="53482624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8857,11 +10929,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118992256"/>
-        <c:axId val="119008640"/>
+        <c:axId val="53532160"/>
+        <c:axId val="53536256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118992256"/>
+        <c:axId val="53532160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8100000"/>
@@ -8918,12 +10990,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119008640"/>
+        <c:crossAx val="53536256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119008640"/>
+        <c:axId val="53536256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -8959,7 +11031,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118992256"/>
+        <c:crossAx val="53532160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10467,6 +12539,1257 @@
 </c:userShapes>
 </file>
 
+<file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>7938</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>464671</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>126587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>464671</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>118649</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing23.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.09397</cdr:x>
+      <cdr:y>0.68146</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.95162</cdr:x>
+      <cdr:y>0.68146</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="5" name="Straight Connector 4"/>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="675415" y="2942271"/>
+          <a:ext cx="6164560" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050"/>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.19256</cdr:x>
+      <cdr:y>0.25093</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.34325</cdr:x>
+      <cdr:y>0.31939</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1387028" y="1107657"/>
+          <a:ext cx="1085442" cy="302199"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>hash</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1" baseline="0"/>
+            <a:t> table size</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t> = 2^21</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.19699</cdr:x>
+      <cdr:y>0.23683</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.19913</cdr:x>
+      <cdr:y>0.89616</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="6" name="Straight Connector 5"/>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
+          <a:off x="1418921" y="1045415"/>
+          <a:ext cx="15432" cy="2910430"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050"/>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.79527</cdr:x>
+      <cdr:y>0.63769</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.94596</cdr:x>
+      <cdr:y>0.70615</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="7" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5728447" y="2814918"/>
+          <a:ext cx="1085442" cy="302199"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>hash</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1" baseline="0"/>
+            <a:t> target performance</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t> = 436</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.63057</cdr:x>
+      <cdr:y>0.25714</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.75752</cdr:x>
+      <cdr:y>0.30622</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="8" name="TextBox 7"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4542117" y="1135062"/>
+          <a:ext cx="914400" cy="216647"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>simple list chaining</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.61791</cdr:x>
+      <cdr:y>0.43238</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.74486</cdr:x>
+      <cdr:y>0.48146</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="9" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4437250" y="1897189"/>
+          <a:ext cx="911591" cy="215349"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>cache</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>optimized list chaining [2-item</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1" baseline="0"/>
+            <a:t> linking</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>]</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.73937</cdr:x>
+      <cdr:y>0.56897</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.86632</cdr:x>
+      <cdr:y>0.61805</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="10" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5309459" y="2496537"/>
+          <a:ext cx="911591" cy="215349"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>cache</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>optimized list chaining [3-item</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1" baseline="0"/>
+            <a:t> linking</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>]</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.34723</cdr:x>
+      <cdr:y>0.5903</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.47418</cdr:x>
+      <cdr:y>0.63938</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="11" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2501154" y="2605742"/>
+          <a:ext cx="914400" cy="216647"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>rb-tree collision resolving</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing24.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.09601</cdr:x>
+      <cdr:y>0.60576</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.95366</cdr:x>
+      <cdr:y>0.60576</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="5" name="Straight Connector 4"/>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="689455" y="2657959"/>
+          <a:ext cx="6158799" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050"/>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.19256</cdr:x>
+      <cdr:y>0.25093</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.34325</cdr:x>
+      <cdr:y>0.31939</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1387028" y="1107657"/>
+          <a:ext cx="1085442" cy="302199"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>hash</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1" baseline="0"/>
+            <a:t> table size</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t> = 2^21</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.19699</cdr:x>
+      <cdr:y>0.23683</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.19913</cdr:x>
+      <cdr:y>0.89616</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="6" name="Straight Connector 5"/>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
+          <a:off x="1418921" y="1045415"/>
+          <a:ext cx="15432" cy="2910430"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050"/>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.79119</cdr:x>
+      <cdr:y>0.56199</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.94188</cdr:x>
+      <cdr:y>0.63045</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="7" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5681539" y="2465903"/>
+          <a:ext cx="1082108" cy="300389"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>hash</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1" baseline="0"/>
+            <a:t> target performance</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t> = 5.5M</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.53534</cdr:x>
+      <cdr:y>0.78258</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.66229</cdr:x>
+      <cdr:y>0.83166</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="8" name="TextBox 7"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3844288" y="3433817"/>
+          <a:ext cx="911630" cy="215354"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>simple list chaining</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.73559</cdr:x>
+      <cdr:y>0.77079</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.86253</cdr:x>
+      <cdr:y>0.81987</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="9" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5282310" y="3382092"/>
+          <a:ext cx="911559" cy="215353"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>cache optimized list chaining [2-item</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1" baseline="0"/>
+            <a:t> linking</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>]</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.74005</cdr:x>
+      <cdr:y>0.66582</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.867</cdr:x>
+      <cdr:y>0.7149</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="10" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5314319" y="2921478"/>
+          <a:ext cx="911630" cy="215353"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>cache optimized list chaining [3-item</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1" baseline="0"/>
+            <a:t> linking</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>]</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.29281</cdr:x>
+      <cdr:y>0.63149</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.41976</cdr:x>
+      <cdr:y>0.68057</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="11" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2102695" y="2770850"/>
+          <a:ext cx="911630" cy="215353"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>rb-tree collision resolving</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
@@ -12315,12 +15638,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="15:20" x14ac:dyDescent="0.35">
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
     </row>
     <row r="3" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O3" t="s">
@@ -12523,12 +15846,12 @@
       </c>
     </row>
     <row r="31" spans="16:26" x14ac:dyDescent="0.35">
-      <c r="W31" s="1" t="s">
+      <c r="W31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X31" s="1"/>
-      <c r="Y31" s="1"/>
-      <c r="Z31" s="1"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="2"/>
+      <c r="Z31" s="2"/>
     </row>
     <row r="32" spans="16:26" x14ac:dyDescent="0.35">
       <c r="P32" t="s">
@@ -13076,8 +16399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="M5:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13099,7 +16422,7 @@
       <c r="P5">
         <v>436</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="1">
         <f>R5/N5</f>
         <v>0.67758328627893849</v>
       </c>
@@ -13121,7 +16444,7 @@
       <c r="P6">
         <v>436</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="1">
         <f t="shared" ref="Q6:Q12" si="1">R6/N6</f>
         <v>0.97600650671004474</v>
       </c>
@@ -13143,7 +16466,7 @@
       <c r="P7">
         <v>436</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="Q7" s="1">
         <f t="shared" si="1"/>
         <v>1.949634443541836</v>
       </c>
@@ -13165,7 +16488,7 @@
       <c r="P8">
         <v>436</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="Q8" s="1">
         <f t="shared" si="1"/>
         <v>2.7210884353741496</v>
       </c>
@@ -13187,7 +16510,7 @@
       <c r="P9">
         <v>436</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="Q9" s="1">
         <f t="shared" si="1"/>
         <v>3.6979969183359014</v>
       </c>
@@ -13209,7 +16532,7 @@
       <c r="P10">
         <v>436</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="Q10" s="1">
         <f t="shared" si="1"/>
         <v>5.5684454756380513</v>
       </c>
@@ -13231,7 +16554,7 @@
       <c r="P11">
         <v>436</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="Q11" s="1">
         <f t="shared" si="1"/>
         <v>6.3829787234042552</v>
       </c>
@@ -13253,7 +16576,7 @@
       <c r="P12">
         <v>436</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="Q12" s="1">
         <f t="shared" si="1"/>
         <v>7.6677316293929714</v>
       </c>
@@ -13294,4 +16617,362 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="N5:W14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N41" sqref="N41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="14" max="14" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="14:23" x14ac:dyDescent="0.35">
+      <c r="O5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>13</v>
+      </c>
+      <c r="S5" t="s">
+        <v>14</v>
+      </c>
+      <c r="U5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="14:23" x14ac:dyDescent="0.35">
+      <c r="N6">
+        <v>100000</v>
+      </c>
+      <c r="O6">
+        <v>311</v>
+      </c>
+      <c r="P6" s="3">
+        <f>W6/O6</f>
+        <v>7.717041800643087</v>
+      </c>
+      <c r="Q6">
+        <v>257</v>
+      </c>
+      <c r="R6" s="3">
+        <f>W6/Q6</f>
+        <v>9.3385214007782107</v>
+      </c>
+      <c r="S6">
+        <v>258</v>
+      </c>
+      <c r="T6" s="3">
+        <f>W6/S6</f>
+        <v>9.3023255813953494</v>
+      </c>
+      <c r="U6">
+        <v>259</v>
+      </c>
+      <c r="V6" s="3">
+        <f>W6/U6</f>
+        <v>9.2664092664092657</v>
+      </c>
+      <c r="W6">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="7" spans="14:23" x14ac:dyDescent="0.35">
+      <c r="N7">
+        <v>250000</v>
+      </c>
+      <c r="O7">
+        <v>333</v>
+      </c>
+      <c r="P7" s="3">
+        <f t="shared" ref="P7:P14" si="0">W7/O7</f>
+        <v>7.2072072072072073</v>
+      </c>
+      <c r="Q7">
+        <v>258</v>
+      </c>
+      <c r="R7" s="3">
+        <f t="shared" ref="R7:R14" si="1">W7/Q7</f>
+        <v>9.3023255813953494</v>
+      </c>
+      <c r="S7">
+        <v>261</v>
+      </c>
+      <c r="T7" s="3">
+        <f t="shared" ref="T7:T14" si="2">W7/S7</f>
+        <v>9.1954022988505741</v>
+      </c>
+      <c r="U7">
+        <v>259</v>
+      </c>
+      <c r="V7" s="3">
+        <f t="shared" ref="V7:V14" si="3">W7/U7</f>
+        <v>9.2664092664092657</v>
+      </c>
+      <c r="W7">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="8" spans="14:23" x14ac:dyDescent="0.35">
+      <c r="N8">
+        <v>500000</v>
+      </c>
+      <c r="O8">
+        <v>324</v>
+      </c>
+      <c r="P8" s="3">
+        <f t="shared" si="0"/>
+        <v>7.4074074074074074</v>
+      </c>
+      <c r="Q8">
+        <v>267</v>
+      </c>
+      <c r="R8" s="3">
+        <f t="shared" si="1"/>
+        <v>8.9887640449438209</v>
+      </c>
+      <c r="S8">
+        <v>268</v>
+      </c>
+      <c r="T8" s="3">
+        <f t="shared" si="2"/>
+        <v>8.9552238805970141</v>
+      </c>
+      <c r="U8">
+        <v>269</v>
+      </c>
+      <c r="V8" s="3">
+        <f t="shared" si="3"/>
+        <v>8.921933085501859</v>
+      </c>
+      <c r="W8">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="9" spans="14:23" x14ac:dyDescent="0.35">
+      <c r="N9">
+        <v>750000</v>
+      </c>
+      <c r="O9">
+        <v>357</v>
+      </c>
+      <c r="P9" s="3">
+        <f t="shared" si="0"/>
+        <v>6.7226890756302522</v>
+      </c>
+      <c r="Q9">
+        <v>276</v>
+      </c>
+      <c r="R9" s="3">
+        <f t="shared" si="1"/>
+        <v>8.695652173913043</v>
+      </c>
+      <c r="S9">
+        <v>278</v>
+      </c>
+      <c r="T9" s="3">
+        <f t="shared" si="2"/>
+        <v>8.6330935251798557</v>
+      </c>
+      <c r="U9">
+        <v>281</v>
+      </c>
+      <c r="V9" s="3">
+        <f t="shared" si="3"/>
+        <v>8.5409252669039137</v>
+      </c>
+      <c r="W9">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="10" spans="14:23" x14ac:dyDescent="0.35">
+      <c r="N10">
+        <v>1000000</v>
+      </c>
+      <c r="O10">
+        <v>344</v>
+      </c>
+      <c r="P10" s="3">
+        <f t="shared" si="0"/>
+        <v>6.9767441860465116</v>
+      </c>
+      <c r="Q10">
+        <v>278</v>
+      </c>
+      <c r="R10" s="3">
+        <f t="shared" si="1"/>
+        <v>8.6330935251798557</v>
+      </c>
+      <c r="S10">
+        <v>284</v>
+      </c>
+      <c r="T10" s="3">
+        <f t="shared" si="2"/>
+        <v>8.4507042253521121</v>
+      </c>
+      <c r="U10">
+        <v>292</v>
+      </c>
+      <c r="V10" s="3">
+        <f t="shared" si="3"/>
+        <v>8.2191780821917817</v>
+      </c>
+      <c r="W10">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="11" spans="14:23" x14ac:dyDescent="0.35">
+      <c r="N11">
+        <v>2000000</v>
+      </c>
+      <c r="O11">
+        <v>398</v>
+      </c>
+      <c r="P11" s="3">
+        <f t="shared" si="0"/>
+        <v>6.0301507537688446</v>
+      </c>
+      <c r="Q11">
+        <v>314</v>
+      </c>
+      <c r="R11" s="3">
+        <f t="shared" si="1"/>
+        <v>7.6433121019108281</v>
+      </c>
+      <c r="S11">
+        <v>314</v>
+      </c>
+      <c r="T11" s="3">
+        <f t="shared" si="2"/>
+        <v>7.6433121019108281</v>
+      </c>
+      <c r="U11">
+        <v>330</v>
+      </c>
+      <c r="V11" s="3">
+        <f t="shared" si="3"/>
+        <v>7.2727272727272725</v>
+      </c>
+      <c r="W11">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="12" spans="14:23" x14ac:dyDescent="0.35">
+      <c r="N12">
+        <v>4000000</v>
+      </c>
+      <c r="O12">
+        <v>518</v>
+      </c>
+      <c r="P12" s="3">
+        <f t="shared" si="0"/>
+        <v>4.6332046332046328</v>
+      </c>
+      <c r="Q12">
+        <v>350</v>
+      </c>
+      <c r="R12" s="3">
+        <f t="shared" si="1"/>
+        <v>6.8571428571428568</v>
+      </c>
+      <c r="S12">
+        <v>369</v>
+      </c>
+      <c r="T12" s="3">
+        <f t="shared" si="2"/>
+        <v>6.5040650406504064</v>
+      </c>
+      <c r="U12">
+        <v>397</v>
+      </c>
+      <c r="V12" s="3">
+        <f t="shared" si="3"/>
+        <v>6.0453400503778338</v>
+      </c>
+      <c r="W12">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="13" spans="14:23" x14ac:dyDescent="0.35">
+      <c r="N13">
+        <v>8000000</v>
+      </c>
+      <c r="O13">
+        <v>743</v>
+      </c>
+      <c r="P13" s="3">
+        <f t="shared" si="0"/>
+        <v>3.2301480484522207</v>
+      </c>
+      <c r="Q13">
+        <v>438</v>
+      </c>
+      <c r="R13" s="3">
+        <f t="shared" si="1"/>
+        <v>5.4794520547945202</v>
+      </c>
+      <c r="S13">
+        <v>468</v>
+      </c>
+      <c r="T13" s="3">
+        <f t="shared" si="2"/>
+        <v>5.1282051282051286</v>
+      </c>
+      <c r="U13">
+        <v>492</v>
+      </c>
+      <c r="V13" s="3">
+        <f t="shared" si="3"/>
+        <v>4.8780487804878048</v>
+      </c>
+      <c r="W13">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="14" spans="14:23" x14ac:dyDescent="0.35">
+      <c r="N14">
+        <v>16000000</v>
+      </c>
+      <c r="O14">
+        <v>881</v>
+      </c>
+      <c r="P14" s="3">
+        <f t="shared" si="0"/>
+        <v>2.7241770715096481</v>
+      </c>
+      <c r="Q14">
+        <v>591</v>
+      </c>
+      <c r="R14" s="3">
+        <f t="shared" si="1"/>
+        <v>4.0609137055837561</v>
+      </c>
+      <c r="S14">
+        <v>668</v>
+      </c>
+      <c r="T14" s="3">
+        <f t="shared" si="2"/>
+        <v>3.5928143712574849</v>
+      </c>
+      <c r="U14">
+        <v>625</v>
+      </c>
+      <c r="V14" s="3">
+        <f t="shared" si="3"/>
+        <v>3.84</v>
+      </c>
+      <c r="W14">
+        <v>2400</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
parallel processing description and charts added
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="110" windowWidth="14360" windowHeight="4680" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="360" yWindow="110" windowWidth="14360" windowHeight="4680" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Ideal NAT" sheetId="3" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="tree_hash" sheetId="10" r:id="rId7"/>
     <sheet name="hash-size dependancy" sheetId="11" r:id="rId8"/>
     <sheet name="hash_table comparison" sheetId="12" r:id="rId9"/>
+    <sheet name="parallel_with_opt_hash" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -106,13 +107,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,11 +353,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="120612352"/>
-        <c:axId val="120615296"/>
+        <c:axId val="114707456"/>
+        <c:axId val="114743168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="120612352"/>
+        <c:axId val="114707456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -373,7 +375,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="120615296"/>
+        <c:crossAx val="114743168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -381,7 +383,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="120615296"/>
+        <c:axId val="114743168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -406,7 +408,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="120612352"/>
+        <c:crossAx val="114707456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1126,11 +1128,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="54240384"/>
-        <c:axId val="54242304"/>
+        <c:axId val="121289728"/>
+        <c:axId val="121304192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54240384"/>
+        <c:axId val="121289728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16100000.000000002"/>
@@ -1187,12 +1189,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54242304"/>
+        <c:crossAx val="121304192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54242304"/>
+        <c:axId val="121304192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -1229,7 +1231,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54240384"/>
+        <c:crossAx val="121289728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2002,11 +2004,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="54378496"/>
-        <c:axId val="54380416"/>
+        <c:axId val="121161216"/>
+        <c:axId val="121163136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54378496"/>
+        <c:axId val="121161216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16200000.000000002"/>
@@ -2063,12 +2065,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54380416"/>
+        <c:crossAx val="121163136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54380416"/>
+        <c:axId val="121163136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -2105,7 +2107,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54378496"/>
+        <c:crossAx val="121161216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2505,11 +2507,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="54270976"/>
-        <c:axId val="54299648"/>
+        <c:axId val="121369344"/>
+        <c:axId val="121639680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54270976"/>
+        <c:axId val="121369344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16100000.000000002"/>
@@ -2566,12 +2568,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54299648"/>
+        <c:crossAx val="121639680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54299648"/>
+        <c:axId val="121639680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2607,7 +2609,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54270976"/>
+        <c:crossAx val="121369344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2944,11 +2946,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="54430720"/>
-        <c:axId val="54454528"/>
+        <c:axId val="121697024"/>
+        <c:axId val="121462784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="54430720"/>
+        <c:axId val="121697024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3003,7 +3005,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54454528"/>
+        <c:crossAx val="121462784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3011,7 +3013,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54454528"/>
+        <c:axId val="121462784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3047,7 +3049,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54430720"/>
+        <c:crossAx val="121697024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3384,11 +3386,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="53735808"/>
-        <c:axId val="53736960"/>
+        <c:axId val="121499648"/>
+        <c:axId val="121502720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="53735808"/>
+        <c:axId val="121499648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3443,7 +3445,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53736960"/>
+        <c:crossAx val="121502720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3451,7 +3453,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53736960"/>
+        <c:axId val="121502720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3487,7 +3489,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53735808"/>
+        <c:crossAx val="121499648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4404,11 +4406,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="58435456"/>
-        <c:axId val="57335168"/>
+        <c:axId val="121980800"/>
+        <c:axId val="122003456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58435456"/>
+        <c:axId val="121980800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4463,12 +4465,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57335168"/>
+        <c:crossAx val="122003456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57335168"/>
+        <c:axId val="122003456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="900"/>
@@ -4505,7 +4507,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58435456"/>
+        <c:crossAx val="121980800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5454,11 +5456,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="83141376"/>
-        <c:axId val="83143296"/>
+        <c:axId val="122038912"/>
+        <c:axId val="122065664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83141376"/>
+        <c:axId val="122038912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5513,12 +5515,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83143296"/>
+        <c:crossAx val="122065664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83143296"/>
+        <c:axId val="122065664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -5554,7 +5556,975 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83141376"/>
+        <c:crossAx val="122038912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln cmpd="sng">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr anchor="t" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0"/>
+              <a:t>Nat Performance - Hash-based NAT table</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>CPU: i5-4210U, 4 cores</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="800" b="1"/>
+              <a:t>[cycles/packet]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.9126195079782243E-2"/>
+          <c:y val="2.1070705564572093E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.4863324687894712E-2"/>
+          <c:y val="0.23883489800482879"/>
+          <c:w val="0.8587591963900808"/>
+          <c:h val="0.66316192505535121"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>target_performance</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FCD184"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_hash!$O$4:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_hash!$P$4:$P$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>436</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>1_core</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.8276689661826426E-2"/>
+                  <c:y val="1.5572430164270132E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.2150007236239071E-2"/>
+                  <c:y val="2.0055330282961092E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="500"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_with_opt_hash!$P$6:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_with_opt_hash!$R$6:$R$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5.825242718446602</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3811659192825116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7971014492753623</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.3811659192825116</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.7692307692307692</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.9850374064837908</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.9259259259259256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5813953488372094</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.8289738430583498</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.1811846689895473</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>2_core</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.3681677842635921E-2"/>
+                  <c:y val="-1.8049320725912133E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="500"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_with_opt_hash!$P$6:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_with_opt_hash!$S$6:$S$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.8360655737704921</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.8360655737704921</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.3023255813953494</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.1603053435114496</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.7560975609756095</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6021505376344081</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.022556390977444</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.8560885608856097</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.6330935251798557</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.4507042253521121</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>3_core</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.5623040185247721E-2"/>
+                  <c:y val="1.1089530045579093E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="500"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_with_opt_hash!$P$6:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_with_opt_hash!$T$6:$T$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>12.060301507537689</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.182741116751268</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.619469026548673</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.435233160621761</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.435233160621761</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.435233160621761</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.435233160621761</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.307692307692308</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.594202898550725</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>4_core</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.496478363645134E-3"/>
+                  <c:y val="1.1089530045579134E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="500"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>parallel_with_opt_hash!$P$6:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>parallel_with_opt_hash!$U$6:$U$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>13.872832369942197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.285714285714286</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.201183431952662</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.457831325301205</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.37125748502994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.201183431952662</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.872832369942197</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.035087719298245</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.37125748502994</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.201183431952662</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="50915968"/>
+        <c:axId val="50348800"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="50915968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="24499999.999999996"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="800" baseline="0"/>
+                  <a:t>network connections [n]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.81805196827046911"/>
+              <c:y val="0.86911217245385308"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="50348800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="50348800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="15"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="22225">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="50915968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6191,11 +7161,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="120571776"/>
-        <c:axId val="120573312"/>
+        <c:axId val="120390784"/>
+        <c:axId val="120407168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="120571776"/>
+        <c:axId val="120390784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2200"/>
@@ -6241,12 +7211,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="120573312"/>
+        <c:crossAx val="120407168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="120573312"/>
+        <c:axId val="120407168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6271,7 +7241,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="120571776"/>
+        <c:crossAx val="120390784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6914,11 +7884,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="53300224"/>
-        <c:axId val="53320704"/>
+        <c:axId val="120435456"/>
+        <c:axId val="120603392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53300224"/>
+        <c:axId val="120435456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2200"/>
@@ -6964,12 +7934,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="53320704"/>
+        <c:crossAx val="120603392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53320704"/>
+        <c:axId val="120603392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6994,7 +7964,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="53300224"/>
+        <c:crossAx val="120435456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7538,11 +8508,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="53619328"/>
-        <c:axId val="53648000"/>
+        <c:axId val="120625024"/>
+        <c:axId val="120645504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53619328"/>
+        <c:axId val="120625024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -7601,12 +8571,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53648000"/>
+        <c:crossAx val="120645504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53648000"/>
+        <c:axId val="120645504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4000000"/>
@@ -7643,7 +8613,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53619328"/>
+        <c:crossAx val="120625024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8088,11 +9058,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="53690368"/>
-        <c:axId val="53692288"/>
+        <c:axId val="120696192"/>
+        <c:axId val="120706560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53690368"/>
+        <c:axId val="120696192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="101000"/>
@@ -8152,12 +9122,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53692288"/>
+        <c:crossAx val="120706560"/>
         <c:crossesAt val="1.0000000000000002E-3"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53692288"/>
+        <c:axId val="120706560"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -8193,7 +9163,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53690368"/>
+        <c:crossAx val="120696192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8877,11 +9847,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="53795072"/>
-        <c:axId val="53813632"/>
+        <c:axId val="120860672"/>
+        <c:axId val="120862592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53795072"/>
+        <c:axId val="120860672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2100000"/>
@@ -8941,12 +9911,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53813632"/>
+        <c:crossAx val="120862592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53813632"/>
+        <c:axId val="120862592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -8982,7 +9952,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53795072"/>
+        <c:crossAx val="120860672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9683,11 +10653,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="53866880"/>
-        <c:axId val="53868800"/>
+        <c:axId val="120915840"/>
+        <c:axId val="120950784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53866880"/>
+        <c:axId val="120915840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2100000"/>
@@ -9747,12 +10717,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53868800"/>
+        <c:crossAx val="120950784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53868800"/>
+        <c:axId val="120950784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -9788,7 +10758,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53866880"/>
+        <c:crossAx val="120915840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10307,11 +11277,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="53482624"/>
-        <c:axId val="53484544"/>
+        <c:axId val="121074048"/>
+        <c:axId val="121086336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53482624"/>
+        <c:axId val="121074048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8100000"/>
@@ -10368,12 +11338,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53484544"/>
+        <c:crossAx val="121086336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53484544"/>
+        <c:axId val="121086336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -10409,7 +11379,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53482624"/>
+        <c:crossAx val="121074048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10929,11 +11899,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="53532160"/>
-        <c:axId val="53536256"/>
+        <c:axId val="120981376"/>
+        <c:axId val="120983552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53532160"/>
+        <c:axId val="120981376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8100000"/>
@@ -10990,12 +11960,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53536256"/>
+        <c:crossAx val="120983552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53536256"/>
+        <c:axId val="120983552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -11031,7 +12001,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53532160"/>
+        <c:crossAx val="120981376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13790,6 +14760,123 @@
 </c:userShapes>
 </file>
 
+<file path=xl/drawings/drawing25.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>395513</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>17236</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing26.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.80851</cdr:x>
+      <cdr:y>0.63225</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.9592</cdr:x>
+      <cdr:y>0.66514</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6727027" y="3620184"/>
+          <a:ext cx="1253788" cy="188325"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="600" b="1"/>
+            <a:t>target performance = 5.5 </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.0955</cdr:x>
+      <cdr:y>0.65777</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.95293</cdr:x>
+      <cdr:y>0.65851</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="3" name="Straight Connector 2"/>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
+          <a:off x="793516" y="3761828"/>
+          <a:ext cx="7124277" cy="4283"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050"/>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
@@ -14692,6 +15779,769 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="P5:Y27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="16" max="16" width="10.453125" customWidth="1"/>
+    <col min="17" max="17" width="10.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="16:25" x14ac:dyDescent="0.35">
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>2</v>
+      </c>
+      <c r="T5">
+        <v>3</v>
+      </c>
+      <c r="U5">
+        <v>4</v>
+      </c>
+      <c r="V5">
+        <v>5</v>
+      </c>
+      <c r="W5">
+        <v>6</v>
+      </c>
+      <c r="X5">
+        <v>7</v>
+      </c>
+      <c r="Y5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="16:25" x14ac:dyDescent="0.35">
+      <c r="P6">
+        <v>100000</v>
+      </c>
+      <c r="Q6">
+        <v>2400</v>
+      </c>
+      <c r="R6" s="2">
+        <f>Q6/R18</f>
+        <v>5.825242718446602</v>
+      </c>
+      <c r="S6" s="2">
+        <f>Q6/S18</f>
+        <v>9.8360655737704921</v>
+      </c>
+      <c r="T6" s="2">
+        <f>Q6/T18</f>
+        <v>12.060301507537689</v>
+      </c>
+      <c r="U6" s="2">
+        <f>Q6/U18</f>
+        <v>13.872832369942197</v>
+      </c>
+      <c r="V6" s="2">
+        <f>Q6/V18</f>
+        <v>16.216216216216218</v>
+      </c>
+      <c r="W6" s="2">
+        <f>Q6/W18</f>
+        <v>18.320610687022899</v>
+      </c>
+      <c r="X6" s="2">
+        <f>Q6/X18</f>
+        <v>21.238938053097346</v>
+      </c>
+      <c r="Y6" s="2">
+        <f>Q6/Y18</f>
+        <v>20.869565217391305</v>
+      </c>
+    </row>
+    <row r="7" spans="16:25" x14ac:dyDescent="0.35">
+      <c r="P7">
+        <v>250000</v>
+      </c>
+      <c r="Q7">
+        <v>2400</v>
+      </c>
+      <c r="R7" s="2">
+        <f t="shared" ref="R7:W7" si="0">Q7/R19</f>
+        <v>5.3811659192825116</v>
+      </c>
+      <c r="S7" s="2">
+        <f t="shared" ref="S7:S15" si="1">Q7/S19</f>
+        <v>9.8360655737704921</v>
+      </c>
+      <c r="T7" s="2">
+        <f t="shared" ref="T7:T15" si="2">Q7/T19</f>
+        <v>12</v>
+      </c>
+      <c r="U7" s="2">
+        <f t="shared" ref="U7:U15" si="3">Q7/U19</f>
+        <v>14.285714285714286</v>
+      </c>
+      <c r="V7" s="2">
+        <f t="shared" ref="V7:V15" si="4">Q7/V19</f>
+        <v>15.09433962264151</v>
+      </c>
+      <c r="W7" s="2">
+        <f t="shared" ref="W7:W15" si="5">Q7/W19</f>
+        <v>17.777777777777779</v>
+      </c>
+      <c r="X7" s="2">
+        <f t="shared" ref="X7:X15" si="6">Q7/X19</f>
+        <v>17.391304347826086</v>
+      </c>
+      <c r="Y7" s="2">
+        <f t="shared" ref="Y7:Y15" si="7">Q7/Y19</f>
+        <v>17.647058823529413</v>
+      </c>
+    </row>
+    <row r="8" spans="16:25" x14ac:dyDescent="0.35">
+      <c r="P8">
+        <v>500000</v>
+      </c>
+      <c r="Q8">
+        <v>2400</v>
+      </c>
+      <c r="R8" s="2">
+        <f t="shared" ref="R8:W8" si="8">Q8/R20</f>
+        <v>5.7971014492753623</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="1"/>
+        <v>9.3023255813953494</v>
+      </c>
+      <c r="T8" s="2">
+        <f t="shared" si="2"/>
+        <v>12.182741116751268</v>
+      </c>
+      <c r="U8" s="2">
+        <f t="shared" si="3"/>
+        <v>14.201183431952662</v>
+      </c>
+      <c r="V8" s="2">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="W8" s="2">
+        <f t="shared" si="5"/>
+        <v>16.107382550335572</v>
+      </c>
+      <c r="X8" s="2">
+        <f t="shared" si="6"/>
+        <v>17.021276595744681</v>
+      </c>
+      <c r="Y8" s="2">
+        <f t="shared" si="7"/>
+        <v>16.783216783216783</v>
+      </c>
+    </row>
+    <row r="9" spans="16:25" x14ac:dyDescent="0.35">
+      <c r="P9">
+        <v>750000</v>
+      </c>
+      <c r="Q9">
+        <v>2400</v>
+      </c>
+      <c r="R9" s="2">
+        <f t="shared" ref="R9:W9" si="9">Q9/R21</f>
+        <v>5.3811659192825116</v>
+      </c>
+      <c r="S9" s="2">
+        <f t="shared" si="1"/>
+        <v>9.1603053435114496</v>
+      </c>
+      <c r="T9" s="2">
+        <f t="shared" si="2"/>
+        <v>10.619469026548673</v>
+      </c>
+      <c r="U9" s="2">
+        <f t="shared" si="3"/>
+        <v>14.457831325301205</v>
+      </c>
+      <c r="V9" s="2">
+        <f t="shared" si="4"/>
+        <v>15.189873417721518</v>
+      </c>
+      <c r="W9" s="2">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="X9" s="2">
+        <f t="shared" si="6"/>
+        <v>15.894039735099337</v>
+      </c>
+      <c r="Y9" s="2">
+        <f t="shared" si="7"/>
+        <v>16.107382550335572</v>
+      </c>
+    </row>
+    <row r="10" spans="16:25" x14ac:dyDescent="0.35">
+      <c r="P10">
+        <v>1000000</v>
+      </c>
+      <c r="Q10">
+        <v>2400</v>
+      </c>
+      <c r="R10" s="2">
+        <f t="shared" ref="R10:W10" si="10">Q10/R22</f>
+        <v>5.7692307692307692</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" si="1"/>
+        <v>9.7560975609756095</v>
+      </c>
+      <c r="T10" s="2">
+        <f t="shared" si="2"/>
+        <v>12.435233160621761</v>
+      </c>
+      <c r="U10" s="2">
+        <f t="shared" si="3"/>
+        <v>14.37125748502994</v>
+      </c>
+      <c r="V10" s="2">
+        <f t="shared" si="4"/>
+        <v>14.634146341463415</v>
+      </c>
+      <c r="W10" s="2">
+        <f t="shared" si="5"/>
+        <v>15.584415584415584</v>
+      </c>
+      <c r="X10" s="2">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="Y10" s="2">
+        <f t="shared" si="7"/>
+        <v>16.107382550335572</v>
+      </c>
+    </row>
+    <row r="11" spans="16:25" x14ac:dyDescent="0.35">
+      <c r="P11">
+        <v>2000000</v>
+      </c>
+      <c r="Q11">
+        <v>2400</v>
+      </c>
+      <c r="R11" s="2">
+        <f t="shared" ref="R11:W11" si="11">Q11/R23</f>
+        <v>5.9850374064837908</v>
+      </c>
+      <c r="S11" s="2">
+        <f t="shared" si="1"/>
+        <v>8.6021505376344081</v>
+      </c>
+      <c r="T11" s="2">
+        <f t="shared" si="2"/>
+        <v>12.435233160621761</v>
+      </c>
+      <c r="U11" s="2">
+        <f t="shared" si="3"/>
+        <v>14.201183431952662</v>
+      </c>
+      <c r="V11" s="2">
+        <f t="shared" si="4"/>
+        <v>14.545454545454545</v>
+      </c>
+      <c r="W11" s="2">
+        <f t="shared" si="5"/>
+        <v>14.723926380368098</v>
+      </c>
+      <c r="X11" s="2">
+        <f t="shared" si="6"/>
+        <v>15.384615384615385</v>
+      </c>
+      <c r="Y11" s="2">
+        <f t="shared" si="7"/>
+        <v>15.09433962264151</v>
+      </c>
+    </row>
+    <row r="12" spans="16:25" x14ac:dyDescent="0.35">
+      <c r="P12">
+        <v>4000000</v>
+      </c>
+      <c r="Q12">
+        <v>2400</v>
+      </c>
+      <c r="R12" s="2">
+        <f t="shared" ref="R12:W12" si="12">Q12/R24</f>
+        <v>5.9259259259259256</v>
+      </c>
+      <c r="S12" s="2">
+        <f t="shared" si="1"/>
+        <v>9.022556390977444</v>
+      </c>
+      <c r="T12" s="2">
+        <f t="shared" si="2"/>
+        <v>12.435233160621761</v>
+      </c>
+      <c r="U12" s="2">
+        <f t="shared" si="3"/>
+        <v>13.872832369942197</v>
+      </c>
+      <c r="V12" s="2">
+        <f t="shared" si="4"/>
+        <v>14.117647058823529</v>
+      </c>
+      <c r="W12" s="2">
+        <f t="shared" si="5"/>
+        <v>14.201183431952662</v>
+      </c>
+      <c r="X12" s="2">
+        <f t="shared" si="6"/>
+        <v>14.545454545454545</v>
+      </c>
+      <c r="Y12" s="2">
+        <f t="shared" si="7"/>
+        <v>14.201183431952662</v>
+      </c>
+    </row>
+    <row r="13" spans="16:25" x14ac:dyDescent="0.35">
+      <c r="P13">
+        <v>8000000</v>
+      </c>
+      <c r="Q13">
+        <v>2400</v>
+      </c>
+      <c r="R13" s="2">
+        <f t="shared" ref="R13:W13" si="13">Q13/R25</f>
+        <v>5.5813953488372094</v>
+      </c>
+      <c r="S13" s="2">
+        <f t="shared" si="1"/>
+        <v>8.8560885608856097</v>
+      </c>
+      <c r="T13" s="2">
+        <f t="shared" si="2"/>
+        <v>12.435233160621761</v>
+      </c>
+      <c r="U13" s="2">
+        <f t="shared" si="3"/>
+        <v>14.035087719298245</v>
+      </c>
+      <c r="V13" s="2">
+        <f t="shared" si="4"/>
+        <v>14.117647058823529</v>
+      </c>
+      <c r="W13" s="2">
+        <f t="shared" si="5"/>
+        <v>13.953488372093023</v>
+      </c>
+      <c r="X13" s="2">
+        <f t="shared" si="6"/>
+        <v>14.035087719298245</v>
+      </c>
+      <c r="Y13" s="2">
+        <f t="shared" si="7"/>
+        <v>13.714285714285714</v>
+      </c>
+    </row>
+    <row r="14" spans="16:25" x14ac:dyDescent="0.35">
+      <c r="P14">
+        <v>16000000</v>
+      </c>
+      <c r="Q14">
+        <v>2400</v>
+      </c>
+      <c r="R14" s="2">
+        <f t="shared" ref="R14:W14" si="14">Q14/R26</f>
+        <v>4.8289738430583498</v>
+      </c>
+      <c r="S14" s="2">
+        <f t="shared" si="1"/>
+        <v>8.6330935251798557</v>
+      </c>
+      <c r="T14" s="2">
+        <f t="shared" si="2"/>
+        <v>12.307692307692308</v>
+      </c>
+      <c r="U14" s="2">
+        <f t="shared" si="3"/>
+        <v>14.37125748502994</v>
+      </c>
+      <c r="V14" s="2">
+        <f t="shared" si="4"/>
+        <v>13.793103448275861</v>
+      </c>
+      <c r="W14" s="2">
+        <f t="shared" si="5"/>
+        <v>13.953488372093023</v>
+      </c>
+      <c r="X14" s="2">
+        <f t="shared" si="6"/>
+        <v>13.872832369942197</v>
+      </c>
+      <c r="Y14" s="2">
+        <f t="shared" si="7"/>
+        <v>13.714285714285714</v>
+      </c>
+    </row>
+    <row r="15" spans="16:25" x14ac:dyDescent="0.35">
+      <c r="P15">
+        <v>24000000</v>
+      </c>
+      <c r="Q15">
+        <v>2400</v>
+      </c>
+      <c r="R15" s="2">
+        <f t="shared" ref="R15:W15" si="15">Q15/R27</f>
+        <v>4.1811846689895473</v>
+      </c>
+      <c r="S15" s="2">
+        <f t="shared" si="1"/>
+        <v>8.4507042253521121</v>
+      </c>
+      <c r="T15" s="2">
+        <f t="shared" si="2"/>
+        <v>11.594202898550725</v>
+      </c>
+      <c r="U15" s="2">
+        <f t="shared" si="3"/>
+        <v>14.201183431952662</v>
+      </c>
+      <c r="V15" s="2">
+        <f t="shared" si="4"/>
+        <v>13.953488372093023</v>
+      </c>
+      <c r="W15" s="2">
+        <f t="shared" si="5"/>
+        <v>13.48314606741573</v>
+      </c>
+      <c r="X15" s="2">
+        <f t="shared" si="6"/>
+        <v>13.559322033898304</v>
+      </c>
+      <c r="Y15" s="2">
+        <f t="shared" si="7"/>
+        <v>13.259668508287293</v>
+      </c>
+    </row>
+    <row r="17" spans="17:25" x14ac:dyDescent="0.35">
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>2</v>
+      </c>
+      <c r="T17">
+        <v>3</v>
+      </c>
+      <c r="U17">
+        <v>4</v>
+      </c>
+      <c r="V17">
+        <v>5</v>
+      </c>
+      <c r="W17">
+        <v>6</v>
+      </c>
+      <c r="X17">
+        <v>7</v>
+      </c>
+      <c r="Y17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="17:25" x14ac:dyDescent="0.35">
+      <c r="Q18">
+        <v>100000</v>
+      </c>
+      <c r="R18" s="4">
+        <v>412</v>
+      </c>
+      <c r="S18" s="4">
+        <v>244</v>
+      </c>
+      <c r="T18" s="4">
+        <v>199</v>
+      </c>
+      <c r="U18" s="4">
+        <v>173</v>
+      </c>
+      <c r="V18" s="4">
+        <v>148</v>
+      </c>
+      <c r="W18" s="4">
+        <v>131</v>
+      </c>
+      <c r="X18" s="4">
+        <v>113</v>
+      </c>
+      <c r="Y18" s="4">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="17:25" x14ac:dyDescent="0.35">
+      <c r="Q19">
+        <v>250000</v>
+      </c>
+      <c r="R19" s="4">
+        <v>446</v>
+      </c>
+      <c r="S19" s="4">
+        <v>244</v>
+      </c>
+      <c r="T19" s="4">
+        <v>200</v>
+      </c>
+      <c r="U19" s="4">
+        <v>168</v>
+      </c>
+      <c r="V19" s="4">
+        <v>159</v>
+      </c>
+      <c r="W19" s="4">
+        <v>135</v>
+      </c>
+      <c r="X19" s="4">
+        <v>138</v>
+      </c>
+      <c r="Y19" s="4">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="17:25" x14ac:dyDescent="0.35">
+      <c r="Q20">
+        <v>500000</v>
+      </c>
+      <c r="R20" s="4">
+        <v>414</v>
+      </c>
+      <c r="S20" s="4">
+        <v>258</v>
+      </c>
+      <c r="T20" s="4">
+        <v>197</v>
+      </c>
+      <c r="U20" s="4">
+        <v>169</v>
+      </c>
+      <c r="V20" s="4">
+        <v>160</v>
+      </c>
+      <c r="W20" s="4">
+        <v>149</v>
+      </c>
+      <c r="X20" s="4">
+        <v>141</v>
+      </c>
+      <c r="Y20" s="4">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="17:25" x14ac:dyDescent="0.35">
+      <c r="Q21">
+        <v>750000</v>
+      </c>
+      <c r="R21" s="4">
+        <v>446</v>
+      </c>
+      <c r="S21" s="4">
+        <v>262</v>
+      </c>
+      <c r="T21" s="4">
+        <v>226</v>
+      </c>
+      <c r="U21" s="4">
+        <v>166</v>
+      </c>
+      <c r="V21" s="4">
+        <v>158</v>
+      </c>
+      <c r="W21" s="4">
+        <v>150</v>
+      </c>
+      <c r="X21" s="4">
+        <v>151</v>
+      </c>
+      <c r="Y21" s="4">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="17:25" x14ac:dyDescent="0.35">
+      <c r="Q22">
+        <v>1000000</v>
+      </c>
+      <c r="R22" s="4">
+        <v>416</v>
+      </c>
+      <c r="S22" s="4">
+        <v>246</v>
+      </c>
+      <c r="T22" s="4">
+        <v>193</v>
+      </c>
+      <c r="U22" s="4">
+        <v>167</v>
+      </c>
+      <c r="V22" s="4">
+        <v>164</v>
+      </c>
+      <c r="W22" s="4">
+        <v>154</v>
+      </c>
+      <c r="X22" s="4">
+        <v>150</v>
+      </c>
+      <c r="Y22" s="4">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="17:25" x14ac:dyDescent="0.35">
+      <c r="Q23">
+        <v>2000000</v>
+      </c>
+      <c r="R23" s="4">
+        <v>401</v>
+      </c>
+      <c r="S23" s="4">
+        <v>279</v>
+      </c>
+      <c r="T23" s="4">
+        <v>193</v>
+      </c>
+      <c r="U23" s="4">
+        <v>169</v>
+      </c>
+      <c r="V23" s="4">
+        <v>165</v>
+      </c>
+      <c r="W23" s="4">
+        <v>163</v>
+      </c>
+      <c r="X23" s="4">
+        <v>156</v>
+      </c>
+      <c r="Y23" s="4">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="17:25" x14ac:dyDescent="0.35">
+      <c r="Q24">
+        <v>4000000</v>
+      </c>
+      <c r="R24" s="4">
+        <v>405</v>
+      </c>
+      <c r="S24" s="4">
+        <v>266</v>
+      </c>
+      <c r="T24" s="4">
+        <v>193</v>
+      </c>
+      <c r="U24" s="4">
+        <v>173</v>
+      </c>
+      <c r="V24" s="4">
+        <v>170</v>
+      </c>
+      <c r="W24" s="4">
+        <v>169</v>
+      </c>
+      <c r="X24" s="4">
+        <v>165</v>
+      </c>
+      <c r="Y24" s="4">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="17:25" x14ac:dyDescent="0.35">
+      <c r="Q25">
+        <v>8000000</v>
+      </c>
+      <c r="R25" s="4">
+        <v>430</v>
+      </c>
+      <c r="S25" s="4">
+        <v>271</v>
+      </c>
+      <c r="T25" s="4">
+        <v>193</v>
+      </c>
+      <c r="U25" s="4">
+        <v>171</v>
+      </c>
+      <c r="V25" s="4">
+        <v>170</v>
+      </c>
+      <c r="W25" s="4">
+        <v>172</v>
+      </c>
+      <c r="X25" s="4">
+        <v>171</v>
+      </c>
+      <c r="Y25" s="4">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="17:25" x14ac:dyDescent="0.35">
+      <c r="Q26">
+        <v>16000000</v>
+      </c>
+      <c r="R26" s="4">
+        <v>497</v>
+      </c>
+      <c r="S26" s="4">
+        <v>278</v>
+      </c>
+      <c r="T26" s="4">
+        <v>195</v>
+      </c>
+      <c r="U26" s="4">
+        <v>167</v>
+      </c>
+      <c r="V26" s="4">
+        <v>174</v>
+      </c>
+      <c r="W26" s="4">
+        <v>172</v>
+      </c>
+      <c r="X26" s="4">
+        <v>173</v>
+      </c>
+      <c r="Y26" s="4">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="17:25" x14ac:dyDescent="0.35">
+      <c r="Q27">
+        <v>24000000</v>
+      </c>
+      <c r="R27" s="4">
+        <v>574</v>
+      </c>
+      <c r="S27" s="4">
+        <v>284</v>
+      </c>
+      <c r="T27" s="4">
+        <v>207</v>
+      </c>
+      <c r="U27" s="4">
+        <v>169</v>
+      </c>
+      <c r="V27" s="4">
+        <v>172</v>
+      </c>
+      <c r="W27" s="4">
+        <v>178</v>
+      </c>
+      <c r="X27" s="4">
+        <v>177</v>
+      </c>
+      <c r="Y27" s="4">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="O2:T25"/>
@@ -15627,7 +17477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="O2:Z41"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="R51" sqref="R51"/>
     </sheetView>
   </sheetViews>
@@ -15638,12 +17488,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="15:20" x14ac:dyDescent="0.35">
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
     </row>
     <row r="3" spans="15:20" x14ac:dyDescent="0.35">
       <c r="O3" t="s">
@@ -15846,12 +17696,12 @@
       </c>
     </row>
     <row r="31" spans="16:26" x14ac:dyDescent="0.35">
-      <c r="W31" s="2" t="s">
+      <c r="W31" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="X31" s="2"/>
-      <c r="Y31" s="2"/>
-      <c r="Z31" s="2"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
     </row>
     <row r="32" spans="16:26" x14ac:dyDescent="0.35">
       <c r="P32" t="s">
@@ -16253,8 +18103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="N4:R11"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16623,8 +18473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="N5:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16653,28 +18503,28 @@
       <c r="O6">
         <v>311</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6" s="2">
         <f>W6/O6</f>
         <v>7.717041800643087</v>
       </c>
       <c r="Q6">
         <v>257</v>
       </c>
-      <c r="R6" s="3">
+      <c r="R6" s="2">
         <f>W6/Q6</f>
         <v>9.3385214007782107</v>
       </c>
       <c r="S6">
         <v>258</v>
       </c>
-      <c r="T6" s="3">
+      <c r="T6" s="2">
         <f>W6/S6</f>
         <v>9.3023255813953494</v>
       </c>
       <c r="U6">
         <v>259</v>
       </c>
-      <c r="V6" s="3">
+      <c r="V6" s="2">
         <f>W6/U6</f>
         <v>9.2664092664092657</v>
       </c>
@@ -16689,28 +18539,28 @@
       <c r="O7">
         <v>333</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7" s="2">
         <f t="shared" ref="P7:P14" si="0">W7/O7</f>
         <v>7.2072072072072073</v>
       </c>
       <c r="Q7">
         <v>258</v>
       </c>
-      <c r="R7" s="3">
+      <c r="R7" s="2">
         <f t="shared" ref="R7:R14" si="1">W7/Q7</f>
         <v>9.3023255813953494</v>
       </c>
       <c r="S7">
         <v>261</v>
       </c>
-      <c r="T7" s="3">
+      <c r="T7" s="2">
         <f t="shared" ref="T7:T14" si="2">W7/S7</f>
         <v>9.1954022988505741</v>
       </c>
       <c r="U7">
         <v>259</v>
       </c>
-      <c r="V7" s="3">
+      <c r="V7" s="2">
         <f t="shared" ref="V7:V14" si="3">W7/U7</f>
         <v>9.2664092664092657</v>
       </c>
@@ -16725,28 +18575,28 @@
       <c r="O8">
         <v>324</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8" s="2">
         <f t="shared" si="0"/>
         <v>7.4074074074074074</v>
       </c>
       <c r="Q8">
         <v>267</v>
       </c>
-      <c r="R8" s="3">
+      <c r="R8" s="2">
         <f t="shared" si="1"/>
         <v>8.9887640449438209</v>
       </c>
       <c r="S8">
         <v>268</v>
       </c>
-      <c r="T8" s="3">
+      <c r="T8" s="2">
         <f t="shared" si="2"/>
         <v>8.9552238805970141</v>
       </c>
       <c r="U8">
         <v>269</v>
       </c>
-      <c r="V8" s="3">
+      <c r="V8" s="2">
         <f t="shared" si="3"/>
         <v>8.921933085501859</v>
       </c>
@@ -16761,28 +18611,28 @@
       <c r="O9">
         <v>357</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9" s="2">
         <f t="shared" si="0"/>
         <v>6.7226890756302522</v>
       </c>
       <c r="Q9">
         <v>276</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R9" s="2">
         <f t="shared" si="1"/>
         <v>8.695652173913043</v>
       </c>
       <c r="S9">
         <v>278</v>
       </c>
-      <c r="T9" s="3">
+      <c r="T9" s="2">
         <f t="shared" si="2"/>
         <v>8.6330935251798557</v>
       </c>
       <c r="U9">
         <v>281</v>
       </c>
-      <c r="V9" s="3">
+      <c r="V9" s="2">
         <f t="shared" si="3"/>
         <v>8.5409252669039137</v>
       </c>
@@ -16797,28 +18647,28 @@
       <c r="O10">
         <v>344</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10" s="2">
         <f t="shared" si="0"/>
         <v>6.9767441860465116</v>
       </c>
       <c r="Q10">
         <v>278</v>
       </c>
-      <c r="R10" s="3">
+      <c r="R10" s="2">
         <f t="shared" si="1"/>
         <v>8.6330935251798557</v>
       </c>
       <c r="S10">
         <v>284</v>
       </c>
-      <c r="T10" s="3">
+      <c r="T10" s="2">
         <f t="shared" si="2"/>
         <v>8.4507042253521121</v>
       </c>
       <c r="U10">
         <v>292</v>
       </c>
-      <c r="V10" s="3">
+      <c r="V10" s="2">
         <f t="shared" si="3"/>
         <v>8.2191780821917817</v>
       </c>
@@ -16833,28 +18683,28 @@
       <c r="O11">
         <v>398</v>
       </c>
-      <c r="P11" s="3">
+      <c r="P11" s="2">
         <f t="shared" si="0"/>
         <v>6.0301507537688446</v>
       </c>
       <c r="Q11">
         <v>314</v>
       </c>
-      <c r="R11" s="3">
+      <c r="R11" s="2">
         <f t="shared" si="1"/>
         <v>7.6433121019108281</v>
       </c>
       <c r="S11">
         <v>314</v>
       </c>
-      <c r="T11" s="3">
+      <c r="T11" s="2">
         <f t="shared" si="2"/>
         <v>7.6433121019108281</v>
       </c>
       <c r="U11">
         <v>330</v>
       </c>
-      <c r="V11" s="3">
+      <c r="V11" s="2">
         <f t="shared" si="3"/>
         <v>7.2727272727272725</v>
       </c>
@@ -16869,28 +18719,28 @@
       <c r="O12">
         <v>518</v>
       </c>
-      <c r="P12" s="3">
+      <c r="P12" s="2">
         <f t="shared" si="0"/>
         <v>4.6332046332046328</v>
       </c>
       <c r="Q12">
         <v>350</v>
       </c>
-      <c r="R12" s="3">
+      <c r="R12" s="2">
         <f t="shared" si="1"/>
         <v>6.8571428571428568</v>
       </c>
       <c r="S12">
         <v>369</v>
       </c>
-      <c r="T12" s="3">
+      <c r="T12" s="2">
         <f t="shared" si="2"/>
         <v>6.5040650406504064</v>
       </c>
       <c r="U12">
         <v>397</v>
       </c>
-      <c r="V12" s="3">
+      <c r="V12" s="2">
         <f t="shared" si="3"/>
         <v>6.0453400503778338</v>
       </c>
@@ -16905,28 +18755,28 @@
       <c r="O13">
         <v>743</v>
       </c>
-      <c r="P13" s="3">
+      <c r="P13" s="2">
         <f t="shared" si="0"/>
         <v>3.2301480484522207</v>
       </c>
       <c r="Q13">
         <v>438</v>
       </c>
-      <c r="R13" s="3">
+      <c r="R13" s="2">
         <f t="shared" si="1"/>
         <v>5.4794520547945202</v>
       </c>
       <c r="S13">
         <v>468</v>
       </c>
-      <c r="T13" s="3">
+      <c r="T13" s="2">
         <f t="shared" si="2"/>
         <v>5.1282051282051286</v>
       </c>
       <c r="U13">
         <v>492</v>
       </c>
-      <c r="V13" s="3">
+      <c r="V13" s="2">
         <f t="shared" si="3"/>
         <v>4.8780487804878048</v>
       </c>
@@ -16941,28 +18791,28 @@
       <c r="O14">
         <v>881</v>
       </c>
-      <c r="P14" s="3">
+      <c r="P14" s="2">
         <f t="shared" si="0"/>
         <v>2.7241770715096481</v>
       </c>
       <c r="Q14">
         <v>591</v>
       </c>
-      <c r="R14" s="3">
+      <c r="R14" s="2">
         <f t="shared" si="1"/>
         <v>4.0609137055837561</v>
       </c>
       <c r="S14">
         <v>668</v>
       </c>
-      <c r="T14" s="3">
+      <c r="T14" s="2">
         <f t="shared" si="2"/>
         <v>3.5928143712574849</v>
       </c>
       <c r="U14">
         <v>625</v>
       </c>
-      <c r="V14" s="3">
+      <c r="V14" s="2">
         <f t="shared" si="3"/>
         <v>3.84</v>
       </c>

</xml_diff>